<commit_message>
Update on Growth Rate simulations
</commit_message>
<xml_diff>
--- a/Data/ZeLa Data/specific_rates_R.xlsx
+++ b/Data/ZeLa Data/specific_rates_R.xlsx
@@ -10,8 +10,6 @@
     <sheet name="Specific Rates" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Avg_U1_U3" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Avg_U4_U8" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Int_U1_U3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Int_U4_U8" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -8057,2660 +8055,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AK7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Interval</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>3-hydroxybutyric acid</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>NH4</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>SGR</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>acetic acid</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>alanine</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>arginine</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>asparagine</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>aspartic acid</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>butyric &amp; 2-hydroxy- butyric acids</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>citric acid</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>cystine</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>ethanol</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>formic acid</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>fumaric acid</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>glucose</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>glutamic acid</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>glutamine</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>glycine</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>histidine</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>hydroxyproline</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>isoleucine</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>isovaleric acid</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>lactic acid</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>leucine</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>malic acid</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>methionine</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>phenylalanine</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>proline</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>pyroglutamic acid</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>pyruvic acid</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>serine</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>threonine</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>tryptophan</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>tyrosine</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>valine</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>P0 to P2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>(0.008166499479549545, 0.010538516927805419)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>(0.321016430908764, 0.3521318544936917)</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>(0.03477980097000294, 0.03668187178298088)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>(0.012450547223100766, 0.020620970658455626)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>(0.14046639786670356, 0.15073771073833608)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>(-0.027104150004720915, -0.012724844097729674)</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>(-0.2441802629425836, -0.14916650200471326)</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>(0.021706969875753997, 0.04423510271625481)</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>(0.011067839094043918, 0.011349987516805861)</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>(-0.01370313594453831, -0.007923956111640304)</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>(0.029424179215691855, 0.08247128201308557)</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>(0.08179229248314811, 0.09153532064364724)</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>(-1.0309829532522248, 0.2643057960946525)</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>(0.010115572650876932, 0.039037379023549916)</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>(-0.6125761713360117, -0.48123396488504444)</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>(0.025569190723151194, 0.02987724606411261)</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>(-0.01085692232398086, -0.0013477609466165073)</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>(-0.009678163576330516, -0.003858017777885262)</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>(-0.0213235834284352, -0.012262758083600975)</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>(1.5188837248771934, 1.7019619514173108)</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>(-0.035410761070565476, -0.0222656764949959)</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>(-0.0399183559061049, -0.015431981346213411)</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>(-0.01336653352863121, -0.009763246659852775)</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>(-0.004915450064346785, 0.006717517781747199)</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>(0.05739146278590467, 0.12616356298608586)</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>(0.23572391616759772, 0.2850912461599499)</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>(-0.078689769576754, -0.06157688050838914)</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>(-0.1755518651588202, -0.09407384895843907)</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>(-0.026325795675623355, -0.007283765217360251)</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>(-0.009662196639530203, -0.005583473724542766)</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>(0.007879001270544458, 0.012746790756435086)</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>(-0.02941897601205555, -0.018804792220122525)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>P12 to P14</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(-8.39546132537721e-05, 4.560812670552097e-05)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>(-0.0005482014186594601, 0.0009586915739328136)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>(-0.007542422712027455, 0.0035840628745758265)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>(-0.011192818883999629, 0.006657606756716167)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>(-0.0015887023928546262, 0.00018519876712457992)</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>(-0.0002177100482620783, 0.00011009119537185955)</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>(-0.0001729015384511131, 0.00045380598894689394)</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>(-1.2144957480793252e-05, 3.402790963493942e-05)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>(-9.601912407452855e-05, 0.0003261944625434407)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>(-0.0006811175908184038, 0.0019050736244145177)</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>(-0.0002661670095933984, 0.0007724695496843109)</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>(-0.00014674303515176888, 4.474158796631919e-05)</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>(-0.014387511225125578, 0.03359397456896264)</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>(-6.815770532846231e-05, 9.961039859034785e-05)</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>(-3.5612031780356806e-05, 4.542816748428538e-06)</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>(-0.001142649470583699, 0.0007065715138663782)</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>(-3.649689760848444e-05, 3.128706189465842e-05)</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>(-0.0004992163641956536, 0.00030943417703228806)</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>(-1.6890244344463573e-06, 2.161891017612375e-05)</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>(3.111465607480232e-06, 5.960356924606487e-05)</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>(-0.023183824948553783, 0.009785320605924096)</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>(-7.549949336471446e-05, 4.677563884062115e-05)</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>(-0.00013600351076928463, 0.00013931992152483617)</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>(-0.00024945394806296896, 8.511137281109325e-05)</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>(-8.789520188321216e-05, 4.476861579723963e-05)</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>(-2.287218839921593e-06, 1.1118700737464837e-05)</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>(-0.00047952502848397284, 0.00031522890000287417)</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>(-2.2550890739553493e-06, 0.0009132326831841919)</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>(-0.0005267763957316298, 9.40090200288994e-05)</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>(-0.0001993194589596273, 4.597219860025995e-05)</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>(-0.00021772930992070398, 0.00013051502465676764)</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>(-1.2131608981341694e-05, 6.025821132265216e-06)</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>(-1.681696757487691e-05, 3.179320870664153e-05)</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>(1.73093222859375e-05, 3.409320952736023e-05)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>P2 to P4</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(0.0029663969974917134, 0.0040307836038947255)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>(0.0850646354705032, 0.10960108026654826)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>(0.0326349974145016, 0.035864607666101986)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(0.0010005870662509017, 0.0014213738361694653)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>(0.04414108899846242, 0.05275002632266158)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>(-0.017891958282831563, -0.013804977694288479)</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>(-0.10229536348340487, -0.0868133895404255)</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>(0.013437437277154874, 0.01942634780174117)</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>(0.001054194796294079, 0.001524305648832723)</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>(0.0054900565158512195, 0.007045685892599738)</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>(-0.003518306867980612, -0.003002091792068283)</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>(0.015008408180773185, 0.06817045121995913)</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>(0.025181308050919633, 0.029164243977463932)</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>(-0.00015288601180831992, 0.0005705783638352253)</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>(-0.5526513172781969, -0.44990636591780164)</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>(0.009251111650394616, 0.014667570063583327)</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>(-0.10475736664494283, -0.09647687227121439)</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>(0.010642981982146908, 0.014438989972383989)</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>(-0.006403321405500352, -0.005434202476254297)</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>(-0.003826362971354376, -0.0006198258802103675)</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>(-0.015169563290087156, -0.012133950584715853)</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>(6.922897133027506e-05, 0.000967505214093092)</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>(0.665746454037536, 0.7511988219190959)</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>(-0.02466488326724021, -0.020542183729683184)</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>(-0.025133231527083303, -0.020033236056976354)</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>(-0.007763818840533552, -0.006843900334591512)</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>(-0.009411453116721395, -0.008257352131328497)</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>(-0.03991029391861151, -0.02910272933079095)</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>(0.0046370735883056, 0.014663399876445556)</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>(0.002248478143393675, 0.0047866790141344855)</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>(-0.06166853086250897, -0.0509951339946794)</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>(-0.024398733829863725, -0.01084925072051919)</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>(-0.0036532823117856376, -0.00290514556308097)</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>(-0.010821231052590877, -0.009753499738660045)</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>(-0.019906819565754148, -0.017513121253977883)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>P4 to P6</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(0.00033437626319793187, 0.00043751600702068605)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>(-0.004493349444409627, -0.0020290393209418597)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>(0.015759187042837196, 0.018010251694238397)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>(0.005308101248658888, 0.007065947460938929)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>(0.0019250102790020086, 0.005002535742745286)</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>(-0.003968354814250555, -0.003175695531510725)</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>(-0.017053025638559073, -0.012371711886062725)</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>(-0.0016148245587910943, -0.0013368199733820622)</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>(0.0009939611980830049, 0.0010956448712068666)</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>(0.0021437430686616662, 0.0024591564730115155)</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>(-0.0003609369751164402, -0.00028371639802318287)</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>(-0.014494685112728679, 0.018797314416631943)</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>(0.007464488244096922, 0.00892619523821676)</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>(-9.494293375543921e-05, 9.85067796105679e-05)</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>(-0.15262527211729848, -0.09076134030760874)</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>(0.0004595800738029872, 0.0016484232418387033)</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>(-0.0054522789014024966, -0.0039264274487831605)</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>(0.004469134332679223, 0.005593262141223152)</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>(-0.0016169162788435643, -0.001442064514724082)</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>(-0.0009689198159735414, -0.00015311683530337542)</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>(-0.004750126814635226, -0.003528922834954101)</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>(0.0008283639655643022, 0.0009132416700084563)</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>(0.05362351634990829, 0.09079861401515744)</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>(-0.007447942820465959, -0.005536634310884913)</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>(-0.0053599186634632565, -0.004110908709005217)</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>(-0.0017903743516354753, -0.0014301879092741582)</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>(-0.0028936247993936537, -0.0020936418169675763)</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>(-0.005674977665097626, -0.0042307743492844205)</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>(-7.036901305722287e-05, 0.0019212277068652568)</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>(-0.005166123709541615, -0.0039455084543701165)</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>(-0.017481515775144042, -0.013897439661493587)</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>(-0.005012837982868983, -0.0026889170352232443)</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>(-0.0013600737557550476, -0.0011783053196112202)</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t>(-0.001595804359904634, -0.0013534389060469885)</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>(-0.005462725847727822, -0.004123286351532368)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>P6 to P8</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>(-7.973698797207622e-05, 1.8781642894060807e-05)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>(-0.0012460791459115107, -0.00029125495905579687)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>(-0.002750971486459342, -0.0009006623895201169)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>(-0.003864829817702425, -0.0010983479671741183)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>(0.00027227430113478104, 0.0014342490833255267)</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>(4.279315973888379e-05, 0.00017582122595044558)</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>(0.0002007906404284579, 0.0006013660197080774)</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>(0.00011468200423823589, 0.0003636024155801739)</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>(-0.00016475239578599577, -5.843018606419492e-05)</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>(-0.00018837650754805594, -6.985696748275705e-05)</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>(7.16267588628887e-06, 2.1801599061604607e-05)</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>(-0.0008510410490446591, 0.0013556588669471552)</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>(-0.00015607475890765598, -3.966476058886209e-05)</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>(-1.4364304977464906e-05, -9.468993172846771e-06)</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>(0.0028341699043242744, 0.023693314193781678)</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>(-4.447553077636474e-05, 9.2270162126263e-05)</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>(-8.995802961712128e-06, 2.4104181388602668e-06)</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>(-0.00026054091715198703, -6.974900423082074e-06)</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>(3.500472104946645e-06, 0.00010206935745882636)</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>(-3.5658791081325836e-05, 2.595723203949253e-06)</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>(8.490471667259552e-05, 0.00028432453200344387)</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>(-0.00022792538431899094, -0.00010517571586018822)</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>(-0.0164870983840588, 0.0035037024990138875)</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>(0.00016160701212959653, 0.00047122105890778617)</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>(8.527156103289632e-05, 0.0002112178911619311)</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>(2.833138545270915e-05, 0.0001035501982296194)</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>(4.6272682561958993e-05, 0.00013165369293187908)</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>(3.5390095151862584e-05, 0.0002758381097157742)</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>(-0.00016354849141821386, -4.506140738886502e-05)</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>(2.8601906817045925e-05, 9.892314071489225e-05)</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>(0.000214150626375055, 0.0006630843283828662)</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>(-5.98217952512898e-06, 0.00010128920937167043)</t>
-        </is>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>(3.182060051408382e-05, 0.00015012282466393334)</t>
-        </is>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>(2.8689780478248507e-05, 0.00014088668669400613)</t>
-        </is>
-      </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>(9.563711900809563e-05, 0.00028619382475597577)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>P8 to P12</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>(-0.0006042397441733097, -0.00040928477493169774)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>(-0.003917952122895883, 0.00809542802477466)</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>(-0.012412405488411493, -0.004577246866356622)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>(-0.0474459771551989, -0.022674554715703725)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>(-0.01096227407199968, 0.0028618915910895385)</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>(9.226969832415468e-05, 0.000387844304220933)</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>(3.2523939614685185e-06, 8.089589173969943e-05)</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>(0.0011318901175290611, 0.00498451873076248)</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>(-0.0007312717942245547, -0.00021200173895846171)</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>(0.0003511172350594964, 0.0010344910665738226)</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>(0.00014588093253506081, 0.0030851191377430556)</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>(0.0003558397681274945, 0.004357917189281836)</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>(-0.0009518519361848747, -0.00015246717429584283)</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>(0.04810238423237592, 0.21342763896423536)</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>(-0.0030237629714169323, 0.000612217546194696)</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>(-0.00016450871634805675, -4.967020756130497e-05)</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>(-0.0036046066735916957, 0.00020921591744692573)</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>(8.77816516509396e-06, 9.126713904618195e-05)</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>(-6.886278216425602e-05, 0.00035094582447713703)</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>(-2.1177397560108468e-05, 0.0018056200456312566)</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>(-0.001955823208891295, 0.00030451482587271785)</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>(-0.10640311634397945, -0.08737737836967413)</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>(-0.00019094036573375742, 0.002409996038609436)</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>(-1.6494920466751114e-05, 0.0004588628108736386)</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>(-0.0029876167105867624, -0.0004176746872480181)</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>(0.00010163492864865095, 0.00025375933672322395)</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>(0.00017740162254732184, 0.0005035613072832357)</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>(0.000329967867921792, 0.0010707911652638783)</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>(-0.004024298715878696, 0.0004856097222872228)</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>(-0.0011500155724315283, -0.00010574744073406307)</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>(-0.0006057088746739254, 0.00018603299740796344)</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t>(-0.0009887334688317207, 0.0009276074256399597)</t>
-        </is>
-      </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>(0.0003958417246874361, 0.0006568721249208517)</t>
-        </is>
-      </c>
-      <c r="AJ7" t="inlineStr">
-        <is>
-          <t>(-7.379541812601579e-05, 8.703587386317335e-06)</t>
-        </is>
-      </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>(-3.387807652501602e-05, 0.0013910977543392807)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:AK7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Interval</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>3-hydroxybutyric acid</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>NH4</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>SGR</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>acetic acid</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>alanine</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>arginine</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>asparagine</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>aspartic acid</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>butyric &amp; 2-hydroxy- butyric acids</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>citric acid</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>cystine</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>ethanol</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>formic acid</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>fumaric acid</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>glucose</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>glutamic acid</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>glutamine</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>glycine</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>histidine</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>hydroxyproline</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>isoleucine</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>isovaleric acid</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>lactic acid</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>leucine</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>lysine</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>malic acid</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>methionine</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>phenylalanine</t>
-        </is>
-      </c>
-      <c r="AD1" s="1" t="inlineStr">
-        <is>
-          <t>proline</t>
-        </is>
-      </c>
-      <c r="AE1" s="1" t="inlineStr">
-        <is>
-          <t>pyroglutamic acid</t>
-        </is>
-      </c>
-      <c r="AF1" s="1" t="inlineStr">
-        <is>
-          <t>pyruvic acid</t>
-        </is>
-      </c>
-      <c r="AG1" s="1" t="inlineStr">
-        <is>
-          <t>serine</t>
-        </is>
-      </c>
-      <c r="AH1" s="1" t="inlineStr">
-        <is>
-          <t>threonine</t>
-        </is>
-      </c>
-      <c r="AI1" s="1" t="inlineStr">
-        <is>
-          <t>tryptophan</t>
-        </is>
-      </c>
-      <c r="AJ1" s="1" t="inlineStr">
-        <is>
-          <t>tyrosine</t>
-        </is>
-      </c>
-      <c r="AK1" s="1" t="inlineStr">
-        <is>
-          <t>valine</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="inlineStr">
-        <is>
-          <t>P0 to P2</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>(0.32142122582209964, 0.3955191720259801)</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>(0.03290039606854243, 0.03774957566811849)</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>(0.023637513865361687, 0.03051345721183509)</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>(0.14552964754888634, 0.19247243095024621)</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>(-0.032769447508176494, -0.014133675881040891)</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>(-0.3436811824412233, -0.2431223321219481)</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>(0.016370816222320568, 0.04107004888910351)</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>(0.006298411257661982, 0.012718977855163894)</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>(-0.014876158504053286, -0.012172165941449035)</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>(0.005289087977062845, 0.8874203794833273)</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>(0.09771832690473908, 0.11628225365468356)</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>(-0.26908285700356777, 0.11401581413955741)</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>(0.005991729022510108, 0.03321104983121098)</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>(-0.5960436975544523, -0.44221974237143713)</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>(0.033219850974215925, 0.04416954125306821)</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>(-0.017673132822898528, -0.00468656667055203)</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>(-0.019603434109533587, 0.0015699781775511418)</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>(-0.03901893334923635, -0.0077515829576249445)</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>(-0.06027932903441437, -0.016085338652542035)</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>(-0.04079435337022452, -0.01990467616358883)</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>(-0.0216200570805848, -0.011521174058763467)</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>(-0.011786215688011484, 0.0073953214860528775)</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>(0.0027090716148083227, 0.14284093868878295)</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>(0.2335785051819454, 0.33031475937168725)</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>(0.05272640989736213, 0.09649749952949752)</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>(-0.21637004356260006, -0.1319462938056203)</t>
-        </is>
-      </c>
-      <c r="AH2" t="inlineStr">
-        <is>
-          <t>(-0.049034317896795826, -0.020481256669774895)</t>
-        </is>
-      </c>
-      <c r="AI2" t="inlineStr">
-        <is>
-          <t>(-0.008061652582016573, -0.003593377394479105)</t>
-        </is>
-      </c>
-      <c r="AJ2" t="inlineStr">
-        <is>
-          <t>(-0.018860621722477718, 0.0032283854839092897)</t>
-        </is>
-      </c>
-      <c r="AK2" t="inlineStr">
-        <is>
-          <t>(-0.04369581233491087, -0.014722152743653785)</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>P12 to P14</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>(-6.520720605478819e-06, 9.468575336255312e-06)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>(-0.0009868776298975388, 0.0005176365574131498)</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>(-0.010062194632355132, 0.006299474887889614)</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>(-0.010043687075421444, 0.005655876804457177)</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>(-0.0001445657156317638, 6.598378543547296e-05)</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>(-0.00021296345434291554, 0.00013156491666864266)</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>(-0.00015697589967629406, 0.0001148443152691395)</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>(-0.00013100621924267558, 8.243381658366205e-05)</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>(-0.0001806129022946938, 0.00010418757150825263)</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>(-0.00012180436456785441, 0.0005620266650980578)</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>(-0.00026525218232955906, 0.00032451430817893016)</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>(-2.3376746810496142e-05, 1.0627925822847402e-05)</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>(-0.0175580338009638, 0.024630604123566362)</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>(-0.0008429445275380072, 0.00047544050410362293)</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>(-6.986098591856563e-05, 3.1990733525305225e-05)</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>(-0.00158027575939257, 0.0008727609855615255)</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>(-8.783323875783154e-05, 3.565781894263268e-05)</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>(-0.0003609780910086422, 0.0001684310340278591)</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>(-0.00018507321954781413, 0.00025850021745225525)</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>(-0.0007894328987175423, 0.0003985042079530292)</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>(-0.00028687744449023335, 0.00019003186747163718)</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>(-0.0002077539984860827, 0.00037440682279877294)</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>(-0.00011701223174124352, 0.00010757971040330875)</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>(-0.0006664037773293114, 0.00028267651199293106)</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>(-5.905333892255831e-06, 2.149808262186462e-05)</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>(-6.694648965981193e-05, 3.269955930059327e-05)</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>(-3.135953716541235e-05, 9.353847432660161e-05)</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
-        <is>
-          <t>(-0.0033431514871701106, 0.0018019442455307992)</t>
-        </is>
-      </c>
-      <c r="AF3" t="inlineStr">
-        <is>
-          <t>(-5.844367738151745e-05, 0.0002549736519275589)</t>
-        </is>
-      </c>
-      <c r="AG3" t="inlineStr">
-        <is>
-          <t>(-0.00025109925516845566, 0.00012848233883017425)</t>
-        </is>
-      </c>
-      <c r="AH3" t="inlineStr">
-        <is>
-          <t>(-0.000671268619604818, 0.00035625437057995135)</t>
-        </is>
-      </c>
-      <c r="AI3" t="inlineStr">
-        <is>
-          <t>(-7.616189768828141e-05, 0.00013770200395920435)</t>
-        </is>
-      </c>
-      <c r="AJ3" t="inlineStr">
-        <is>
-          <t>(-2.716419764260716e-05, 1.0809588212270463e-05)</t>
-        </is>
-      </c>
-      <c r="AK3" t="inlineStr">
-        <is>
-          <t>(-0.00011786232664567507, 0.00014280181670998454)</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="inlineStr">
-        <is>
-          <t>P2 to P4</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>(-2.847428224023437e-05, -1.8635387077897906e-05)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>(0.10221165201955007, 0.14554488853597383)</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>(0.03309354293725934, 0.03725896271642408)</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>(0.002638267319632167, 0.00488626710775767)</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>(0.07637225350946851, 0.08158474854164972)</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>(-0.01857679552686262, -0.01296370832534256)</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>(-0.12175922854931916, -0.09847188101228786)</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>(0.009224539247103265, 0.015859686721147924)</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>(0.0010922647662979508, 0.0019474035051385992)</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>(0.0058734344015672025, 0.006689186985388617)</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>(-0.004075340882678871, -0.00293636931978161)</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>(-0.09871753880585282, 0.023033090976526928)</t>
-        </is>
-      </c>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>(0.028760778218338914, 0.03360270985055156)</t>
-        </is>
-      </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>(-7.833975441133445e-05, 0.0004872893059172052)</t>
-        </is>
-      </c>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>(-0.42290097983659536, -0.1812331640616548)</t>
-        </is>
-      </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>(0.01025027938754622, 0.016066979043498443)</t>
-        </is>
-      </c>
-      <c r="R4" t="inlineStr">
-        <is>
-          <t>(-0.12103565551864433, -0.09702239568499414)</t>
-        </is>
-      </c>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>(0.015917657554230354, 0.01974320419655635)</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr">
-        <is>
-          <t>(-0.007296228890889772, -0.006488829650645135)</t>
-        </is>
-      </c>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>(-0.003068065897396689, -0.0006777511863598781)</t>
-        </is>
-      </c>
-      <c r="V4" t="inlineStr">
-        <is>
-          <t>(-0.017298818237286878, -0.010429780291920515)</t>
-        </is>
-      </c>
-      <c r="W4" t="inlineStr">
-        <is>
-          <t>(-0.00016817864437160577, 0.000918226502072568)</t>
-        </is>
-      </c>
-      <c r="X4" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>(-0.02665727600464631, -0.017040093324987363)</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>(-0.02604650504073744, -0.021360123882764162)</t>
-        </is>
-      </c>
-      <c r="AA4" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB4" t="inlineStr">
-        <is>
-          <t>(-0.0072970141437743155, -0.00554234080769108)</t>
-        </is>
-      </c>
-      <c r="AC4" t="inlineStr">
-        <is>
-          <t>(-0.01154717610708342, -0.0076168199778974734)</t>
-        </is>
-      </c>
-      <c r="AD4" t="inlineStr">
-        <is>
-          <t>(-0.04248345320699913, -0.02030498373120758)</t>
-        </is>
-      </c>
-      <c r="AE4" t="inlineStr">
-        <is>
-          <t>(0.011678065351912771, 0.019736402514269176)</t>
-        </is>
-      </c>
-      <c r="AF4" t="inlineStr">
-        <is>
-          <t>(0.04339702191595932, 0.055492264820853836)</t>
-        </is>
-      </c>
-      <c r="AG4" t="inlineStr">
-        <is>
-          <t>(-0.07267352333599852, -0.06054709059693089)</t>
-        </is>
-      </c>
-      <c r="AH4" t="inlineStr">
-        <is>
-          <t>(-0.019341620968994576, -0.016115773632365958)</t>
-        </is>
-      </c>
-      <c r="AI4" t="inlineStr">
-        <is>
-          <t>(-0.004206720800954874, -0.002562379347318941)</t>
-        </is>
-      </c>
-      <c r="AJ4" t="inlineStr">
-        <is>
-          <t>(-0.009448271363886127, -0.005338495224258505)</t>
-        </is>
-      </c>
-      <c r="AK4" t="inlineStr">
-        <is>
-          <t>(-0.020348835306287817, -0.01340394173244519)</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>P4 to P6</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>(-1.5916980168386086e-05, 0.00021137894054762489)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>(-0.025255454138806633, -0.014853772506163033)</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>(0.012047606507514207, 0.018563977057166503)</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>(0.0025590723285295763, 0.00334051532103934)</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>(-0.0034831043895964635, 0.029761811684020017)</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>(-0.004658563066113831, -0.0019823726421481377)</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>(-0.018923765280038578, -0.004874475896335067)</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>(-0.0024075661495029017, -0.0015697924357859125)</t>
-        </is>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>(0.0006715308753891579, 0.0014582207473458455)</t>
-        </is>
-      </c>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>(0.0014005408417138777, 0.0020933478108368458)</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>(-0.0004417420610149911, -0.000123024107491422)</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
-          <t>(-0.004178136458239472, 0.0049399333372060735)</t>
-        </is>
-      </c>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>(0.004364713240907194, 0.009123367169027872)</t>
-        </is>
-      </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>(7.502727315465426e-06, 0.00010406035344433581)</t>
-        </is>
-      </c>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>(-0.12136907526419634, -0.06015116704545205)</t>
-        </is>
-      </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>(0.0003062395000899887, 0.0009507544355000697)</t>
-        </is>
-      </c>
-      <c r="R5" t="inlineStr">
-        <is>
-          <t>(-0.010772557563591722, -0.00072425385969784)</t>
-        </is>
-      </c>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>(0.00423661626232545, 0.0072613888070514766)</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr">
-        <is>
-          <t>(-0.0017266833605287595, -0.0007215372645922753)</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>(-0.00033090622435905093, 0.00022043358315017962)</t>
-        </is>
-      </c>
-      <c r="V5" t="inlineStr">
-        <is>
-          <t>(-0.005635681584520595, -0.003023373118328657)</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>(0.0010767518031109488, 0.0013401950859692575)</t>
-        </is>
-      </c>
-      <c r="X5" t="inlineStr">
-        <is>
-          <t>(0.0013738453351346972, 0.0029974855739840793)</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>(-0.008446901704468534, -0.004391667336862805)</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>(-0.0056965559420813, -0.002548711659279077)</t>
-        </is>
-      </c>
-      <c r="AA5" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB5" t="inlineStr">
-        <is>
-          <t>(-0.001823632950249218, -0.0008952377370370567)</t>
-        </is>
-      </c>
-      <c r="AC5" t="inlineStr">
-        <is>
-          <t>(-0.0027244761882574448, -0.0013524449993627201)</t>
-        </is>
-      </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>(-0.004783969285539301, -0.0022753510300530418)</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>(0.0017898996705400468, 0.003082839894334093)</t>
-        </is>
-      </c>
-      <c r="AF5" t="inlineStr">
-        <is>
-          <t>(-0.014477980505565367, -0.011826196818357266)</t>
-        </is>
-      </c>
-      <c r="AG5" t="inlineStr">
-        <is>
-          <t>(-0.016973690218714303, -0.006514747040805553)</t>
-        </is>
-      </c>
-      <c r="AH5" t="inlineStr">
-        <is>
-          <t>(-0.00348730748838464, -0.0019082181744719613)</t>
-        </is>
-      </c>
-      <c r="AI5" t="inlineStr">
-        <is>
-          <t>(-0.0011818515300284279, -0.000714326713516101)</t>
-        </is>
-      </c>
-      <c r="AJ5" t="inlineStr">
-        <is>
-          <t>(-0.002074073703809823, -0.0009593464751419444)</t>
-        </is>
-      </c>
-      <c r="AK5" t="inlineStr">
-        <is>
-          <t>(-0.005880661129811897, -0.003113832057239827)</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>P6 to P8</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>(-5.771076352237273e-05, 1.1523220615663722e-05)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>(0.001876908618764905, 0.003992166779120109)</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>(0.00370763437071568, 0.007324063298029265)</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>(0.0012895815110821602, 0.0024093140917863963)</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>(-0.008762175045417476, -0.002708459848622031)</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>(-0.0006622569617422661, -0.00030150738105654733)</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>(-0.0012946147654787946, -0.0007625658243530294)</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>(-0.0009873549519781631, -0.0004553881605764902)</t>
-        </is>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>(0.00014200906654186817, 0.000290872027474958)</t>
-        </is>
-      </c>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>(0.0002443808710688906, 0.0005912082823727178)</t>
-        </is>
-      </c>
-      <c r="L6" t="inlineStr">
-        <is>
-          <t>(-4.699815715460635e-05, -2.6912975207010315e-05)</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>(-0.0006053784939257312, 0.0009118592307167852)</t>
-        </is>
-      </c>
-      <c r="N6" t="inlineStr">
-        <is>
-          <t>(0.0007106656800930564, 0.0017022760483770764)</t>
-        </is>
-      </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>(2.0399389905120695e-06, 3.271080654348143e-05)</t>
-        </is>
-      </c>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>(-0.029479248871306894, -0.017096152090042192)</t>
-        </is>
-      </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>(0.0004644855883026517, 0.0007776242012140927)</t>
-        </is>
-      </c>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>(-0.000120428615447738, -3.550557454098506e-05)</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>(0.0010539114962596088, 0.0019569441171942196)</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr">
-        <is>
-          <t>(-0.0002074464345235366, -8.918891903544459e-05)</t>
-        </is>
-      </c>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>(5.080498393391226e-05, 0.00018630639582552206)</t>
-        </is>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>(-0.0011300894367558595, -0.0006351336689047764)</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>(0.000698471073762496, 0.0011706155876109185)</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>(3.21077837424462e-05, 0.00010516445951058991)</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr">
-        <is>
-          <t>(-0.0019548798366353514, -0.0011125047146759504)</t>
-        </is>
-      </c>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>(-0.0009698206151542057, -0.0004025618818325408)</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="AB6" t="inlineStr">
-        <is>
-          <t>(-0.00030805305643767834, -0.00014442617014064492)</t>
-        </is>
-      </c>
-      <c r="AC6" t="inlineStr">
-        <is>
-          <t>(-0.00038544205320072226, -0.00020737636896533414)</t>
-        </is>
-      </c>
-      <c r="AD6" t="inlineStr">
-        <is>
-          <t>(-0.0008833873612090337, -0.0002798007334791137)</t>
-        </is>
-      </c>
-      <c r="AE6" t="inlineStr">
-        <is>
-          <t>(0.00045358305682387224, 0.0011002074954193188)</t>
-        </is>
-      </c>
-      <c r="AF6" t="inlineStr">
-        <is>
-          <t>(-0.0006159132376867225, -0.00011629521730175166)</t>
-        </is>
-      </c>
-      <c r="AG6" t="inlineStr">
-        <is>
-          <t>(-0.0020748860567795483, -0.001071863128990361)</t>
-        </is>
-      </c>
-      <c r="AH6" t="inlineStr">
-        <is>
-          <t>(-0.0006077938057656662, -0.00029293354179016416)</t>
-        </is>
-      </c>
-      <c r="AI6" t="inlineStr">
-        <is>
-          <t>(-0.0003227556137818848, -0.00015529092942501656)</t>
-        </is>
-      </c>
-      <c r="AJ6" t="inlineStr">
-        <is>
-          <t>(-0.00034944377757841654, -0.0001542203613581315)</t>
-        </is>
-      </c>
-      <c r="AK6" t="inlineStr">
-        <is>
-          <t>(-0.0011372331768038646, -0.0006204121311568926)</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>P8 to P12</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>(-9.268635572723239e-05, -1.1245986090935542e-05)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>(-0.0023324816362193385, -0.0008798235255725082)</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>(-0.008707456283579409, -0.002937781247612042)</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>(-0.012569070615353716, -0.0037066147996727087)</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>(-0.00044048398486488656, -5.769911236564319e-06)</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>(-0.00021090430295663343, 4.1233254404311016e-05)</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>(-8.13785410763523e-06, 2.7855216285062976e-05)</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>(0.0006174590831356256, 0.0019669174992209496)</t>
-        </is>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>(-0.0006029993732018713, -0.00017184188997214353)</t>
-        </is>
-      </c>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>(-8.296522091894037e-05, 8.456550605412343e-05)</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>(0.0, 0.0)</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>(0.00030542506497996695, 0.0022948153721223485)</t>
-        </is>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>(0.0001625787219967029, 0.0007265949251628497)</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>(-0.00019536333650756893, -3.2063021052162015e-05)</t>
-        </is>
-      </c>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>(0.02126994414856681, 0.07087367579398138)</t>
-        </is>
-      </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>(-0.0016493022420456644, -7.388813922253328e-05)</t>
-        </is>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>(-7.373503938456802e-05, -3.182885519399301e-06)</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>(-0.002989873691417444, -0.0007341966876625232)</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr">
-        <is>
-          <t>(-8.371755607819705e-05, 3.0078333327532997e-05)</t>
-        </is>
-      </c>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>(-0.00017403798565344714, 6.335306780686174e-05)</t>
-        </is>
-      </c>
-      <c r="V7" t="inlineStr">
-        <is>
-          <t>(0.0004414606922316211, 0.0013561747631702953)</t>
-        </is>
-      </c>
-      <c r="W7" t="inlineStr">
-        <is>
-          <t>(-0.001929358345626545, -0.000642668667454384)</t>
-        </is>
-      </c>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>(-0.0014704641028177217, -0.00032432520324388806)</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>(0.0006544385446804906, 0.001956711537100905)</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>(-0.00024037208997418233, -2.898391078272764e-06)</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>(-0.0006095324471212599, -3.6578157880316786e-05)</t>
-        </is>
-      </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>(3.476603088712148e-05, 0.00014515579996807147)</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>(4.313619662297329e-05, 0.00016905225295647613)</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>(-0.0004607189570341941, 4.8711193311980466e-05)</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>(-0.003375881798028882, -0.0010239839895690521)</t>
-        </is>
-      </c>
-      <c r="AF7" t="inlineStr">
-        <is>
-          <t>(-0.0002543015776197495, -6.730521269868896e-05)</t>
-        </is>
-      </c>
-      <c r="AG7" t="inlineStr">
-        <is>
-          <t>(-0.000369862965430046, 5.7632690252000014e-05)</t>
-        </is>
-      </c>
-      <c r="AH7" t="inlineStr">
-        <is>
-          <t>(4.6145652124048514e-05, 0.0004260025234959059)</t>
-        </is>
-      </c>
-      <c r="AI7" t="inlineStr">
-        <is>
-          <t>(0.0002194148170348379, 0.0006026932474802826)</t>
-        </is>
-      </c>
-      <c r="AJ7" t="inlineStr">
-        <is>
-          <t>(-9.2882989198787e-06, 8.82118249217497e-05)</t>
-        </is>
-      </c>
-      <c r="AK7" t="inlineStr">
-        <is>
-          <t>(0.0003339732556027363, 0.0009779888375546642)</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updates on contextualized models and COSMIC-dFBA
</commit_message>
<xml_diff>
--- a/Data/ZeLa Data/specific_rates_R.xlsx
+++ b/Data/ZeLa Data/specific_rates_R.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Specific Rates" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Avg_U1_U3" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Avg_U4_U8" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Specific Rates" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg_U1_U3" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg_U4_U8" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Int_U1_U3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Int_U4_U8" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -19,10 +20,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -39,7 +48,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -48,46 +57,76 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin"/>
       <right style="thin"/>
-      <top/>
+      <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -452,7 +491,7 @@
   </sheetPr>
   <dimension ref="A1:AL49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -6252,16 +6291,16 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A2:A7"/>
     <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="A20:A25"/>
     <mergeCell ref="A26:A31"/>
-    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A32:A37"/>
     <mergeCell ref="A38:A43"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A14:A19"/>
     <mergeCell ref="A44:A49"/>
-    <mergeCell ref="A32:A37"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -6280,194 +6319,194 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Interval</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>3-hydroxybutyric acid</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>NH4</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>SGR</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>acetic acid</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>alanine</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>arginine</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>asparagine</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>aspartic acid</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>butyric &amp; 2-hydroxy- butyric acids</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>citric acid</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>cystine</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>ethanol</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>formic acid</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>fumaric acid</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>glutamic acid</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>glutamine</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>glycine</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>histidine</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>hydroxyproline</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>isoleucine</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>isovaleric acid</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>lactic acid</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>leucine</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>lysine</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>malic acid</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>methionine</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>phenylalanine</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>proline</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AE1" s="4" t="inlineStr">
         <is>
           <t>pyroglutamic acid</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AF1" s="4" t="inlineStr">
         <is>
           <t>pyruvic acid</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AG1" s="4" t="inlineStr">
         <is>
           <t>serine</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AH1" s="4" t="inlineStr">
         <is>
           <t>threonine</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AI1" s="4" t="inlineStr">
         <is>
           <t>tryptophan</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AJ1" s="4" t="inlineStr">
         <is>
           <t>tyrosine</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AK1" s="4" t="inlineStr">
         <is>
           <t>valine</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>P0 to P2</t>
         </is>
@@ -6582,7 +6621,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>P12 to P14</t>
         </is>
@@ -6697,7 +6736,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>P2 to P4</t>
         </is>
@@ -6812,7 +6851,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>P4 to P6</t>
         </is>
@@ -6927,7 +6966,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>P6 to P8</t>
         </is>
@@ -7042,7 +7081,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>P8 to P12</t>
         </is>
@@ -7176,194 +7215,194 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Interval</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>3-hydroxybutyric acid</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>NH4</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>SGR</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>acetic acid</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>alanine</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>arginine</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>asparagine</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>aspartic acid</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>butyric &amp; 2-hydroxy- butyric acids</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>citric acid</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>cystine</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>ethanol</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>formic acid</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>fumaric acid</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>glutamic acid</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>glutamine</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>glycine</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>histidine</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>hydroxyproline</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>isoleucine</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>isovaleric acid</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>lactic acid</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>leucine</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>lysine</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>malic acid</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>methionine</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>phenylalanine</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>proline</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AE1" s="4" t="inlineStr">
         <is>
           <t>pyroglutamic acid</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AF1" s="4" t="inlineStr">
         <is>
           <t>pyruvic acid</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AG1" s="4" t="inlineStr">
         <is>
           <t>serine</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AH1" s="4" t="inlineStr">
         <is>
           <t>threonine</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AI1" s="4" t="inlineStr">
         <is>
           <t>tryptophan</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AJ1" s="4" t="inlineStr">
         <is>
           <t>tyrosine</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="AK1" s="4" t="inlineStr">
         <is>
           <t>valine</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="4" t="inlineStr">
         <is>
           <t>P0 to P2</t>
         </is>
@@ -7478,7 +7517,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="4" t="inlineStr">
         <is>
           <t>P12 to P14</t>
         </is>
@@ -7593,7 +7632,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="4" t="inlineStr">
         <is>
           <t>P2 to P4</t>
         </is>
@@ -7708,7 +7747,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="4" t="inlineStr">
         <is>
           <t>P4 to P6</t>
         </is>
@@ -7823,7 +7862,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="4" t="inlineStr">
         <is>
           <t>P6 to P8</t>
         </is>
@@ -7938,7 +7977,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="4" t="inlineStr">
         <is>
           <t>P8 to P12</t>
         </is>
@@ -8050,6 +8089,2662 @@
       </c>
       <c r="AK7" t="n">
         <v>0.0006559810465787002</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AK7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Interval</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>3-hydroxybutyric acid</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>NH4</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>SGR</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>acetic acid</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>alanine</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>arginine</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>asparagine</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>aspartic acid</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>butyric &amp; 2-hydroxy- butyric acids</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>citric acid</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>cystine</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>ethanol</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>formic acid</t>
+        </is>
+      </c>
+      <c r="O1" s="4" t="inlineStr">
+        <is>
+          <t>fumaric acid</t>
+        </is>
+      </c>
+      <c r="P1" s="4" t="inlineStr">
+        <is>
+          <t>glucose</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>glutamic acid</t>
+        </is>
+      </c>
+      <c r="R1" s="4" t="inlineStr">
+        <is>
+          <t>glutamine</t>
+        </is>
+      </c>
+      <c r="S1" s="4" t="inlineStr">
+        <is>
+          <t>glycine</t>
+        </is>
+      </c>
+      <c r="T1" s="4" t="inlineStr">
+        <is>
+          <t>histidine</t>
+        </is>
+      </c>
+      <c r="U1" s="4" t="inlineStr">
+        <is>
+          <t>hydroxyproline</t>
+        </is>
+      </c>
+      <c r="V1" s="4" t="inlineStr">
+        <is>
+          <t>isoleucine</t>
+        </is>
+      </c>
+      <c r="W1" s="4" t="inlineStr">
+        <is>
+          <t>isovaleric acid</t>
+        </is>
+      </c>
+      <c r="X1" s="4" t="inlineStr">
+        <is>
+          <t>lactic acid</t>
+        </is>
+      </c>
+      <c r="Y1" s="4" t="inlineStr">
+        <is>
+          <t>leucine</t>
+        </is>
+      </c>
+      <c r="Z1" s="4" t="inlineStr">
+        <is>
+          <t>lysine</t>
+        </is>
+      </c>
+      <c r="AA1" s="4" t="inlineStr">
+        <is>
+          <t>malic acid</t>
+        </is>
+      </c>
+      <c r="AB1" s="4" t="inlineStr">
+        <is>
+          <t>methionine</t>
+        </is>
+      </c>
+      <c r="AC1" s="4" t="inlineStr">
+        <is>
+          <t>phenylalanine</t>
+        </is>
+      </c>
+      <c r="AD1" s="4" t="inlineStr">
+        <is>
+          <t>proline</t>
+        </is>
+      </c>
+      <c r="AE1" s="4" t="inlineStr">
+        <is>
+          <t>pyroglutamic acid</t>
+        </is>
+      </c>
+      <c r="AF1" s="4" t="inlineStr">
+        <is>
+          <t>pyruvic acid</t>
+        </is>
+      </c>
+      <c r="AG1" s="4" t="inlineStr">
+        <is>
+          <t>serine</t>
+        </is>
+      </c>
+      <c r="AH1" s="4" t="inlineStr">
+        <is>
+          <t>threonine</t>
+        </is>
+      </c>
+      <c r="AI1" s="4" t="inlineStr">
+        <is>
+          <t>tryptophan</t>
+        </is>
+      </c>
+      <c r="AJ1" s="4" t="inlineStr">
+        <is>
+          <t>tyrosine</t>
+        </is>
+      </c>
+      <c r="AK1" s="4" t="inlineStr">
+        <is>
+          <t>valine</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>P0 to P2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>(0.008166499479549545, 0.010538516927805419)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>(0.321016430908764, 0.3521318544936917)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>(0.03477980097000294, 0.03668187178298088)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>(0.012450547223100766, 0.020620970658455626)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>(0.14046639786670356, 0.15073771073833608)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>(-0.027104150004720915, -0.012724844097729674)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>(-0.2441802629425836, -0.14916650200471326)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>(0.021706969875753997, 0.04423510271625481)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>(0.011067839094043918, 0.011349987516805861)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>(-0.01370313594453831, -0.007923956111640304)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>(0.029424179215691855, 0.08247128201308557)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>(0.08179229248314811, 0.09153532064364724)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>(-1.0309829532522248, 0.2643057960946525)</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>(0.010115572650876932, 0.039037379023549916)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>(-0.6125761713360117, -0.48123396488504444)</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>(0.025569190723151194, 0.02987724606411261)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>(-0.01085692232398086, -0.0013477609466165073)</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>(-0.009678163576330516, -0.0038580177778852615)</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>(-0.0213235834284352, -0.012262758083600975)</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>(1.5188837248771934, 1.7019619514173108)</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>(-0.035410761070565476, -0.0222656764949959)</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>(-0.0399183559061049, -0.015431981346213411)</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>(-0.01336653352863121, -0.009763246659852775)</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>(-0.004915450064346785, 0.006717517781747199)</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>(0.05739146278590467, 0.12616356298608586)</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>(0.23572391616759772, 0.2850912461599499)</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>(-0.078689769576754, -0.06157688050838914)</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>(-0.1755518651588202, -0.09407384895843907)</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>(-0.026325795675623355, -0.007283765217360251)</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>(-0.009662196639530203, -0.005583473724542766)</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>(0.007879001270544458, 0.012746790756435086)</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>(-0.02941897601205555, -0.018804792220122525)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>P12 to P14</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>(-8.39546132537721e-05, 4.560812670552097e-05)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>(-0.0005482014186594601, 0.0009586915739328136)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>(-0.007542422712027455, 0.0035840628745758265)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>(-0.011192818883999629, 0.006657606756716167)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>(-0.0015887023928546262, 0.00018519876712457992)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>(-0.0002177100482620783, 0.00011009119537185955)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>(-0.0001729015384511131, 0.00045380598894689394)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>(-1.2144957480793252e-05, 3.402790963493942e-05)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>(-9.601912407452855e-05, 0.0003261944625434407)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>(-0.0006811175908184038, 0.0019050736244145177)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>(-0.0002661670095933984, 0.0007724695496843109)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>(-0.00014674303515176888, 4.474158796631919e-05)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>(-0.014387511225125578, 0.03359397456896264)</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>(-6.815770532846231e-05, 9.961039859034785e-05)</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>(-3.5612031780356806e-05, 4.542816748428538e-06)</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>(-0.001142649470583699, 0.0007065715138663782)</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>(-3.649689760848444e-05, 3.128706189465842e-05)</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>(-0.0004992163641956536, 0.00030943417703228806)</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>(-1.6890244344463573e-06, 2.161891017612375e-05)</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>(3.111465607480232e-06, 5.960356924606487e-05)</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>(-0.023183824948553783, 0.009785320605924096)</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>(-7.549949336471446e-05, 4.677563884062115e-05)</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>(-0.00013600351076928463, 0.00013931992152483617)</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>(-0.00024945394806296896, 8.511137281109325e-05)</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>(-8.789520188321216e-05, 4.476861579723963e-05)</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>(-2.287218839921593e-06, 1.1118700737464837e-05)</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>(-0.00047952502848397284, 0.00031522890000287417)</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>(-2.2550890739553493e-06, 0.0009132326831841919)</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>(-0.0005267763957316298, 9.40090200288994e-05)</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>(-0.0001993194589596273, 4.597219860025995e-05)</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>(-0.00021772930992070398, 0.00013051502465676764)</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>(-1.2131608981341694e-05, 6.025821132265216e-06)</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>(-1.681696757487691e-05, 3.179320870664153e-05)</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>(1.73093222859375e-05, 3.409320952736023e-05)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>P2 to P4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(0.0029663969974917134, 0.0040307836038947255)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(0.0850646354705032, 0.10960108026654826)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(0.0326349974145016, 0.035864607666101986)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>(0.0010005870662509017, 0.0014213738361694653)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>(0.04414108899846242, 0.05275002632266158)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>(-0.017891958282831563, -0.013804977694288479)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>(-0.10229536348340487, -0.0868133895404255)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>(0.013437437277154874, 0.01942634780174117)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>(0.001054194796294079, 0.001524305648832723)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>(0.0054900565158512195, 0.007045685892599738)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>(-0.003518306867980612, -0.003002091792068283)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>(0.015008408180773189, 0.06817045121995913)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>(0.025181308050919633, 0.029164243977463932)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>(-0.00015288601180831992, 0.0005705783638352253)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>(-0.5526513172781969, -0.44990636591780164)</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>(0.009251111650394616, 0.014667570063583327)</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>(-0.10475736664494283, -0.09647687227121439)</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>(0.010642981982146908, 0.014438989972383989)</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>(-0.006403321405500352, -0.005434202476254297)</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>(-0.003826362971354376, -0.0006198258802103675)</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>(-0.015169563290087156, -0.012133950584715853)</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>(6.922897133027506e-05, 0.000967505214093092)</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>(0.665746454037536, 0.7511988219190959)</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>(-0.02466488326724021, -0.020542183729683184)</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>(-0.025133231527083303, -0.020033236056976354)</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>(-0.007763818840533552, -0.006843900334591512)</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>(-0.009411453116721395, -0.008257352131328497)</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>(-0.03991029391861151, -0.02910272933079095)</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>(0.0046370735883056, 0.014663399876445556)</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>(0.002248478143393675, 0.0047866790141344855)</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>(-0.06166853086250897, -0.0509951339946794)</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>(-0.024398733829863725, -0.01084925072051919)</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>(-0.0036532823117856376, -0.00290514556308097)</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>(-0.010821231052590877, -0.009753499738660045)</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>(-0.019906819565754148, -0.017513121253977883)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>P4 to P6</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>(0.00033437626319793187, 0.00043751600702068605)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>(-0.004493349444409627, -0.0020290393209418597)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>(0.015759187042837196, 0.018010251694238397)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>(0.005308101248658888, 0.007065947460938929)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>(0.0019250102790020086, 0.005002535742745286)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>(-0.003968354814250555, -0.003175695531510725)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>(-0.017053025638559073, -0.012371711886062725)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>(-0.0016148245587910943, -0.0013368199733820622)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>(0.0009939611980830049, 0.0010956448712068666)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>(0.0021437430686616662, 0.0024591564730115155)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>(-0.0003609369751164402, -0.00028371639802318287)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>(-0.014494685112728679, 0.018797314416631943)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>(0.007464488244096922, 0.00892619523821676)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>(-9.494293375543921e-05, 9.85067796105679e-05)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>(-0.15262527211729848, -0.09076134030760874)</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>(0.0004595800738029872, 0.0016484232418387033)</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>(-0.0054522789014024966, -0.0039264274487831605)</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>(0.004469134332679223, 0.005593262141223152)</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>(-0.0016169162788435643, -0.001442064514724082)</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>(-0.0009689198159735414, -0.00015311683530337542)</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>(-0.004750126814635226, -0.003528922834954101)</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>(0.0008283639655643022, 0.0009132416700084563)</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>(0.05362351634990829, 0.09079861401515744)</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>(-0.007447942820465959, -0.005536634310884913)</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>(-0.0053599186634632565, -0.004110908709005217)</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>(-0.0017903743516354753, -0.0014301879092741582)</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>(-0.0028936247993936537, -0.0020936418169675763)</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>(-0.005674977665097626, -0.0042307743492844205)</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>(-7.036901305722287e-05, 0.0019212277068652568)</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>(-0.005166123709541615, -0.0039455084543701165)</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>(-0.017481515775144042, -0.013897439661493587)</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>(-0.005012837982868983, -0.0026889170352232443)</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>(-0.0013600737557550476, -0.0011783053196112202)</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>(-0.001595804359904634, -0.0013534389060469885)</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>(-0.005462725847727822, -0.004123286351532368)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>P6 to P8</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>(-7.973698797207622e-05, 1.8781642894060807e-05)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>(-0.0012460791459115107, -0.00029125495905579687)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>(-0.002750971486459342, -0.0009006623895201169)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>(-0.003864829817702425, -0.0010983479671741183)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>(0.00027227430113478104, 0.0014342490833255267)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>(4.279315973888379e-05, 0.00017582122595044558)</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>(0.0002007906404284579, 0.0006013660197080774)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>(0.00011468200423823589, 0.0003636024155801739)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>(-0.00016475239578599577, -5.843018606419492e-05)</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>(-0.0001883765075480559, -6.985696748275707e-05)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>(7.16267588628887e-06, 2.1801599061604607e-05)</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>(-0.0008510410490446591, 0.0013556588669471552)</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>(-0.00015607475890765598, -3.966476058886209e-05)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>(-1.4364304977464906e-05, -9.468993172846771e-06)</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>(0.0028341699043242744, 0.023693314193781678)</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>(-4.447553077636474e-05, 9.2270162126263e-05)</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>(-8.995802961712128e-06, 2.4104181388602668e-06)</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>(-0.00026054091715198703, -6.974900423082074e-06)</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>(3.500472104946645e-06, 0.00010206935745882636)</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>(-3.5658791081325836e-05, 2.595723203949253e-06)</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>(8.490471667259552e-05, 0.00028432453200344387)</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>(-0.00022792538431899094, -0.00010517571586018822)</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>(-0.0164870983840588, 0.0035037024990138893)</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>(0.00016160701212959653, 0.00047122105890778617)</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>(8.527156103289632e-05, 0.0002112178911619311)</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>(2.833138545270915e-05, 0.0001035501982296194)</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>(4.6272682561958993e-05, 0.00013165369293187908)</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>(3.5390095151862584e-05, 0.0002758381097157742)</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>(-0.00016354849141821386, -4.506140738886502e-05)</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>(2.8601906817045925e-05, 9.892314071489225e-05)</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>(0.000214150626375055, 0.0006630843283828662)</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>(-5.98217952512898e-06, 0.00010128920937167043)</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>(3.182060051408382e-05, 0.00015012282466393334)</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>(2.8689780478248507e-05, 0.00014088668669400613)</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>(9.563711900809563e-05, 0.00028619382475597577)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>P8 to P12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>(-0.0006042397441733097, -0.00040928477493169774)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>(-0.003917952122895882, 0.00809542802477466)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>(-0.012412405488411493, -0.004577246866356622)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>(-0.0474459771551989, -0.022674554715703725)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>(-0.01096227407199968, 0.0028618915910895385)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>(9.226969832415468e-05, 0.000387844304220933)</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>(3.2523939614685117e-06, 8.089589173969943e-05)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>(0.0011318901175290611, 0.00498451873076248)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>(-0.0007312717942245547, -0.00021200173895846171)</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>(0.0003511172350594964, 0.0010344910665738226)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>(0.00014588093253506081, 0.0030851191377430556)</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>(0.0003558397681274945, 0.004357917189281836)</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>(-0.0009518519361848747, -0.00015246717429584283)</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>(0.04810238423237592, 0.21342763896423536)</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>(-0.0030237629714169323, 0.000612217546194696)</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>(-0.00016450871634805675, -4.967020756130497e-05)</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>(-0.0036046066735916957, 0.00020921591744692573)</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>(8.77816516509396e-06, 9.126713904618195e-05)</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>(-6.886278216425604e-05, 0.0003509458244771371)</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>(-2.1177397560108468e-05, 0.0018056200456312566)</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>(-0.001955823208891295, 0.00030451482587271785)</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>(-0.10640311634397945, -0.08737737836967413)</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>(-0.00019094036573375742, 0.002409996038609436)</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>(-1.6494920466751114e-05, 0.0004588628108736386)</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>(-0.0029876167105867624, -0.0004176746872480181)</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>(0.00010163492864865095, 0.00025375933672322395)</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>(0.00017740162254732184, 0.0005035613072832357)</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>(0.000329967867921792, 0.0010707911652638783)</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>(-0.004024298715878696, 0.0004856097222872228)</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>(-0.0011500155724315283, -0.00010574744073406307)</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>(-0.0006057088746739254, 0.00018603299740796344)</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>(-0.0009887334688317207, 0.0009276074256399598)</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>(0.0003958417246874361, 0.0006568721249208517)</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>(-7.379541812601579e-05, 8.703587386317335e-06)</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>(-3.387807652501602e-05, 0.0013910977543392807)</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:AK7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>Interval</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>3-hydroxybutyric acid</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>NH4</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>SGR</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>acetic acid</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>alanine</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>arginine</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>asparagine</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>aspartic acid</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>butyric &amp; 2-hydroxy- butyric acids</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>citric acid</t>
+        </is>
+      </c>
+      <c r="L1" s="4" t="inlineStr">
+        <is>
+          <t>cystine</t>
+        </is>
+      </c>
+      <c r="M1" s="4" t="inlineStr">
+        <is>
+          <t>ethanol</t>
+        </is>
+      </c>
+      <c r="N1" s="4" t="inlineStr">
+        <is>
+          <t>formic acid</t>
+        </is>
+      </c>
+      <c r="O1" s="4" t="inlineStr">
+        <is>
+          <t>fumaric acid</t>
+        </is>
+      </c>
+      <c r="P1" s="4" t="inlineStr">
+        <is>
+          <t>glucose</t>
+        </is>
+      </c>
+      <c r="Q1" s="4" t="inlineStr">
+        <is>
+          <t>glutamic acid</t>
+        </is>
+      </c>
+      <c r="R1" s="4" t="inlineStr">
+        <is>
+          <t>glutamine</t>
+        </is>
+      </c>
+      <c r="S1" s="4" t="inlineStr">
+        <is>
+          <t>glycine</t>
+        </is>
+      </c>
+      <c r="T1" s="4" t="inlineStr">
+        <is>
+          <t>histidine</t>
+        </is>
+      </c>
+      <c r="U1" s="4" t="inlineStr">
+        <is>
+          <t>hydroxyproline</t>
+        </is>
+      </c>
+      <c r="V1" s="4" t="inlineStr">
+        <is>
+          <t>isoleucine</t>
+        </is>
+      </c>
+      <c r="W1" s="4" t="inlineStr">
+        <is>
+          <t>isovaleric acid</t>
+        </is>
+      </c>
+      <c r="X1" s="4" t="inlineStr">
+        <is>
+          <t>lactic acid</t>
+        </is>
+      </c>
+      <c r="Y1" s="4" t="inlineStr">
+        <is>
+          <t>leucine</t>
+        </is>
+      </c>
+      <c r="Z1" s="4" t="inlineStr">
+        <is>
+          <t>lysine</t>
+        </is>
+      </c>
+      <c r="AA1" s="4" t="inlineStr">
+        <is>
+          <t>malic acid</t>
+        </is>
+      </c>
+      <c r="AB1" s="4" t="inlineStr">
+        <is>
+          <t>methionine</t>
+        </is>
+      </c>
+      <c r="AC1" s="4" t="inlineStr">
+        <is>
+          <t>phenylalanine</t>
+        </is>
+      </c>
+      <c r="AD1" s="4" t="inlineStr">
+        <is>
+          <t>proline</t>
+        </is>
+      </c>
+      <c r="AE1" s="4" t="inlineStr">
+        <is>
+          <t>pyroglutamic acid</t>
+        </is>
+      </c>
+      <c r="AF1" s="4" t="inlineStr">
+        <is>
+          <t>pyruvic acid</t>
+        </is>
+      </c>
+      <c r="AG1" s="4" t="inlineStr">
+        <is>
+          <t>serine</t>
+        </is>
+      </c>
+      <c r="AH1" s="4" t="inlineStr">
+        <is>
+          <t>threonine</t>
+        </is>
+      </c>
+      <c r="AI1" s="4" t="inlineStr">
+        <is>
+          <t>tryptophan</t>
+        </is>
+      </c>
+      <c r="AJ1" s="4" t="inlineStr">
+        <is>
+          <t>tyrosine</t>
+        </is>
+      </c>
+      <c r="AK1" s="4" t="inlineStr">
+        <is>
+          <t>valine</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="inlineStr">
+        <is>
+          <t>P0 to P2</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>(0.32142122582209964, 0.3955191720259801)</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>(0.03290039606854243, 0.03774957566811849)</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>(0.023637513865361687, 0.03051345721183509)</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>(0.14552964754888634, 0.19247243095024621)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>(-0.032769447508176494, -0.014133675881040891)</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>(-0.3436811824412233, -0.2431223321219481)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>(0.016370816222320568, 0.04107004888910351)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>(0.006298411257661982, 0.012718977855163894)</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>(-0.014876158504053286, -0.012172165941449035)</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>(0.005289087977062845, 0.8874203794833273)</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>(0.09771832690473908, 0.11628225365468356)</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>(-0.26908285700356777, 0.11401581413955741)</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>(0.005991729022510108, 0.03321104983121098)</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>(-0.5960436975544523, -0.44221974237143713)</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>(0.033219850974215925, 0.04416954125306821)</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>(-0.017673132822898528, -0.00468656667055203)</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>(-0.019603434109533587, 0.0015699781775511418)</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>(-0.03901893334923635, -0.0077515829576249445)</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>(-0.06027932903441437, -0.016085338652542035)</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>(-0.04079435337022452, -0.01990467616358883)</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>(-0.021620057080584804, -0.011521174058763465)</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>(-0.011786215688011484, 0.0073953214860528775)</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>(0.0027090716148083227, 0.14284093868878295)</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>(0.2335785051819454, 0.33031475937168725)</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>(0.05272640989736213, 0.09649749952949752)</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
+          <t>(-0.21637004356260006, -0.1319462938056203)</t>
+        </is>
+      </c>
+      <c r="AH2" t="inlineStr">
+        <is>
+          <t>(-0.049034317896795826, -0.020481256669774895)</t>
+        </is>
+      </c>
+      <c r="AI2" t="inlineStr">
+        <is>
+          <t>(-0.008061652582016573, -0.003593377394479105)</t>
+        </is>
+      </c>
+      <c r="AJ2" t="inlineStr">
+        <is>
+          <t>(-0.018860621722477718, 0.0032283854839092897)</t>
+        </is>
+      </c>
+      <c r="AK2" t="inlineStr">
+        <is>
+          <t>(-0.04369581233491087, -0.014722152743653785)</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="inlineStr">
+        <is>
+          <t>P12 to P14</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>(-6.520720605478817e-06, 9.46857533625531e-06)</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>(-0.0009868776298975388, 0.0005176365574131498)</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>(-0.010062194632355132, 0.006299474887889614)</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>(-0.010043687075421444, 0.005655876804457177)</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>(-0.0001445657156317638, 6.598378543547296e-05)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>(-0.00021296345434291554, 0.00013156491666864266)</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>(-0.00015697589967629403, 0.00011484431526913948)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>(-0.00013100621924267558, 8.243381658366205e-05)</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>(-0.0001806129022946938, 0.00010418757150825263)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>(-0.00012180436456785441, 0.0005620266650980578)</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>(-0.00026525218232955906, 0.00032451430817893016)</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>(-2.3376746810496142e-05, 1.0627925822847402e-05)</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>(-0.0175580338009638, 0.024630604123566362)</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>(-0.0008429445275380072, 0.00047544050410362293)</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>(-6.986098591856563e-05, 3.1990733525305225e-05)</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>(-0.00158027575939257, 0.0008727609855615255)</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>(-8.783323875783154e-05, 3.565781894263268e-05)</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>(-0.0003609780910086422, 0.0001684310340278591)</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>(-0.00018507321954781413, 0.00025850021745225525)</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>(-0.0007894328987175423, 0.0003985042079530292)</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>(-0.0002868774444902334, 0.00019003186747163718)</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>(-0.0002077539984860827, 0.00037440682279877294)</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>(-0.00011701223174124352, 0.00010757971040330875)</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>(-0.0006664037773293114, 0.00028267651199293106)</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>(-5.905333892255831e-06, 2.149808262186462e-05)</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>(-6.694648965981193e-05, 3.269955930059327e-05)</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>(-3.135953716541235e-05, 9.353847432660161e-05)</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>(-0.0033431514871701106, 0.0018019442455307992)</t>
+        </is>
+      </c>
+      <c r="AF3" t="inlineStr">
+        <is>
+          <t>(-5.844367738151745e-05, 0.0002549736519275589)</t>
+        </is>
+      </c>
+      <c r="AG3" t="inlineStr">
+        <is>
+          <t>(-0.00025109925516845566, 0.00012848233883017425)</t>
+        </is>
+      </c>
+      <c r="AH3" t="inlineStr">
+        <is>
+          <t>(-0.0006712686196048179, 0.00035625437057995124)</t>
+        </is>
+      </c>
+      <c r="AI3" t="inlineStr">
+        <is>
+          <t>(-7.616189768828141e-05, 0.00013770200395920435)</t>
+        </is>
+      </c>
+      <c r="AJ3" t="inlineStr">
+        <is>
+          <t>(-2.716419764260716e-05, 1.0809588212270463e-05)</t>
+        </is>
+      </c>
+      <c r="AK3" t="inlineStr">
+        <is>
+          <t>(-0.00011786232664567507, 0.00014280181670998454)</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>P2 to P4</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>(-2.847428224023437e-05, -1.8635387077897906e-05)</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>(0.10221165201955007, 0.14554488853597383)</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>(0.03309354293725934, 0.03725896271642408)</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>(0.002638267319632167, 0.00488626710775767)</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>(0.07637225350946851, 0.08158474854164972)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>(-0.01857679552686262, -0.01296370832534256)</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>(-0.12175922854931916, -0.09847188101228786)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>(0.009224539247103265, 0.015859686721147924)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>(0.0010922647662979508, 0.0019474035051385992)</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>(0.0058734344015672025, 0.006689186985388617)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>(-0.004075340882678871, -0.00293636931978161)</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>(-0.09871753880585282, 0.023033090976526928)</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>(0.028760778218338914, 0.03360270985055156)</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>(-7.833975441133445e-05, 0.0004872893059172052)</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>(-0.42290097983659536, -0.1812331640616548)</t>
+        </is>
+      </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>(0.010250279387546218, 0.016066979043498443)</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>(-0.12103565551864433, -0.09702239568499414)</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>(0.015917657554230354, 0.01974320419655635)</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>(-0.007296228890889772, -0.006488829650645135)</t>
+        </is>
+      </c>
+      <c r="U4" t="inlineStr">
+        <is>
+          <t>(-0.003068065897396689, -0.0006777511863598781)</t>
+        </is>
+      </c>
+      <c r="V4" t="inlineStr">
+        <is>
+          <t>(-0.017298818237286878, -0.010429780291920515)</t>
+        </is>
+      </c>
+      <c r="W4" t="inlineStr">
+        <is>
+          <t>(-0.00016817864437160577, 0.000918226502072568)</t>
+        </is>
+      </c>
+      <c r="X4" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>(-0.02665727600464631, -0.017040093324987363)</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>(-0.02604650504073744, -0.021360123882764162)</t>
+        </is>
+      </c>
+      <c r="AA4" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB4" t="inlineStr">
+        <is>
+          <t>(-0.0072970141437743155, -0.00554234080769108)</t>
+        </is>
+      </c>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>(-0.01154717610708342, -0.0076168199778974734)</t>
+        </is>
+      </c>
+      <c r="AD4" t="inlineStr">
+        <is>
+          <t>(-0.04248345320699913, -0.02030498373120758)</t>
+        </is>
+      </c>
+      <c r="AE4" t="inlineStr">
+        <is>
+          <t>(0.011678065351912771, 0.019736402514269176)</t>
+        </is>
+      </c>
+      <c r="AF4" t="inlineStr">
+        <is>
+          <t>(0.04339702191595932, 0.055492264820853836)</t>
+        </is>
+      </c>
+      <c r="AG4" t="inlineStr">
+        <is>
+          <t>(-0.07267352333599852, -0.06054709059693089)</t>
+        </is>
+      </c>
+      <c r="AH4" t="inlineStr">
+        <is>
+          <t>(-0.019341620968994576, -0.016115773632365958)</t>
+        </is>
+      </c>
+      <c r="AI4" t="inlineStr">
+        <is>
+          <t>(-0.004206720800954874, -0.002562379347318941)</t>
+        </is>
+      </c>
+      <c r="AJ4" t="inlineStr">
+        <is>
+          <t>(-0.009448271363886127, -0.005338495224258505)</t>
+        </is>
+      </c>
+      <c r="AK4" t="inlineStr">
+        <is>
+          <t>(-0.020348835306287817, -0.01340394173244519)</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>P4 to P6</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>(-1.5916980168386086e-05, 0.00021137894054762489)</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>(-0.025255454138806633, -0.014853772506163033)</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>(0.012047606507514207, 0.018563977057166503)</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>(0.0025590723285295763, 0.00334051532103934)</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>(-0.0034831043895964635, 0.029761811684020017)</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>(-0.004658563066113831, -0.0019823726421481377)</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>(-0.01892376528003858, -0.004874475896335066)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>(-0.0024075661495029017, -0.0015697924357859125)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>(0.0006715308753891579, 0.0014582207473458455)</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>(0.0014005408417138777, 0.0020933478108368458)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>(-0.0004417420610149911, -0.000123024107491422)</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>(-0.004178136458239472, 0.0049399333372060735)</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>(0.004364713240907194, 0.009123367169027872)</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>(7.502727315465426e-06, 0.00010406035344433581)</t>
+        </is>
+      </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>(-0.12136907526419634, -0.06015116704545205)</t>
+        </is>
+      </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>(0.0003062395000899887, 0.0009507544355000697)</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>(-0.010772557563591722, -0.00072425385969784)</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>(0.00423661626232545, 0.0072613888070514766)</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>(-0.0017266833605287595, -0.0007215372645922753)</t>
+        </is>
+      </c>
+      <c r="U5" t="inlineStr">
+        <is>
+          <t>(-0.00033090622435905093, 0.00022043358315017962)</t>
+        </is>
+      </c>
+      <c r="V5" t="inlineStr">
+        <is>
+          <t>(-0.005635681584520595, -0.003023373118328657)</t>
+        </is>
+      </c>
+      <c r="W5" t="inlineStr">
+        <is>
+          <t>(0.0010767518031109488, 0.0013401950859692575)</t>
+        </is>
+      </c>
+      <c r="X5" t="inlineStr">
+        <is>
+          <t>(0.0013738453351346972, 0.0029974855739840793)</t>
+        </is>
+      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>(-0.008446901704468534, -0.004391667336862805)</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>(-0.005696555942081301, -0.0025487116592790766)</t>
+        </is>
+      </c>
+      <c r="AA5" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB5" t="inlineStr">
+        <is>
+          <t>(-0.001823632950249218, -0.0008952377370370567)</t>
+        </is>
+      </c>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>(-0.0027244761882574448, -0.0013524449993627201)</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>(-0.004783969285539301, -0.0022753510300530418)</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
+          <t>(0.0017898996705400468, 0.003082839894334093)</t>
+        </is>
+      </c>
+      <c r="AF5" t="inlineStr">
+        <is>
+          <t>(-0.014477980505565367, -0.011826196818357266)</t>
+        </is>
+      </c>
+      <c r="AG5" t="inlineStr">
+        <is>
+          <t>(-0.016973690218714303, -0.006514747040805553)</t>
+        </is>
+      </c>
+      <c r="AH5" t="inlineStr">
+        <is>
+          <t>(-0.00348730748838464, -0.0019082181744719613)</t>
+        </is>
+      </c>
+      <c r="AI5" t="inlineStr">
+        <is>
+          <t>(-0.0011818515300284279, -0.000714326713516101)</t>
+        </is>
+      </c>
+      <c r="AJ5" t="inlineStr">
+        <is>
+          <t>(-0.002074073703809823, -0.0009593464751419444)</t>
+        </is>
+      </c>
+      <c r="AK5" t="inlineStr">
+        <is>
+          <t>(-0.005880661129811897, -0.003113832057239827)</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="inlineStr">
+        <is>
+          <t>P6 to P8</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>(-5.771076352237273e-05, 1.1523220615663722e-05)</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>(0.001876908618764905, 0.003992166779120109)</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>(0.00370763437071568, 0.007324063298029265)</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>(0.0012895815110821602, 0.0024093140917863963)</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>(-0.008762175045417476, -0.002708459848622031)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>(-0.0006622569617422661, -0.00030150738105654733)</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>(-0.0012946147654787946, -0.0007625658243530294)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>(-0.0009873549519781631, -0.0004553881605764902)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>(0.00014200906654186817, 0.000290872027474958)</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>(0.00024438087106889056, 0.0005912082823727178)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>(-4.699815715460635e-05, -2.6912975207010315e-05)</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>(-0.0006053784939257312, 0.0009118592307167852)</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>(0.0007106656800930564, 0.0017022760483770764)</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>(2.0399389905120695e-06, 3.271080654348143e-05)</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>(-0.029479248871306894, -0.017096152090042192)</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>(0.00046448558830265165, 0.0007776242012140928)</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>(-0.000120428615447738, -3.550557454098506e-05)</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>(0.0010539114962596088, 0.0019569441171942196)</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>(-0.0002074464345235366, -8.918891903544459e-05)</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>(5.080498393391225e-05, 0.00018630639582552206)</t>
+        </is>
+      </c>
+      <c r="V6" t="inlineStr">
+        <is>
+          <t>(-0.0011300894367558595, -0.0006351336689047764)</t>
+        </is>
+      </c>
+      <c r="W6" t="inlineStr">
+        <is>
+          <t>(0.000698471073762496, 0.0011706155876109185)</t>
+        </is>
+      </c>
+      <c r="X6" t="inlineStr">
+        <is>
+          <t>(3.21077837424462e-05, 0.00010516445951058991)</t>
+        </is>
+      </c>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>(-0.0019548798366353514, -0.0011125047146759504)</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>(-0.0009698206151542057, -0.0004025618818325408)</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="AB6" t="inlineStr">
+        <is>
+          <t>(-0.00030805305643767834, -0.00014442617014064492)</t>
+        </is>
+      </c>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>(-0.00038544205320072226, -0.00020737636896533414)</t>
+        </is>
+      </c>
+      <c r="AD6" t="inlineStr">
+        <is>
+          <t>(-0.0008833873612090337, -0.0002798007334791137)</t>
+        </is>
+      </c>
+      <c r="AE6" t="inlineStr">
+        <is>
+          <t>(0.00045358305682387224, 0.0011002074954193188)</t>
+        </is>
+      </c>
+      <c r="AF6" t="inlineStr">
+        <is>
+          <t>(-0.0006159132376867225, -0.00011629521730175166)</t>
+        </is>
+      </c>
+      <c r="AG6" t="inlineStr">
+        <is>
+          <t>(-0.0020748860567795483, -0.001071863128990361)</t>
+        </is>
+      </c>
+      <c r="AH6" t="inlineStr">
+        <is>
+          <t>(-0.0006077938057656662, -0.00029293354179016416)</t>
+        </is>
+      </c>
+      <c r="AI6" t="inlineStr">
+        <is>
+          <t>(-0.0003227556137818848, -0.00015529092942501656)</t>
+        </is>
+      </c>
+      <c r="AJ6" t="inlineStr">
+        <is>
+          <t>(-0.00034944377757841654, -0.0001542203613581315)</t>
+        </is>
+      </c>
+      <c r="AK6" t="inlineStr">
+        <is>
+          <t>(-0.0011372331768038646, -0.0006204121311568926)</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="inlineStr">
+        <is>
+          <t>P8 to P12</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>(-9.268635572723239e-05, -1.1245986090935535e-05)</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>(-0.0023324816362193385, -0.0008798235255725082)</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>(-0.008707456283579409, -0.002937781247612042)</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>(-0.012569070615353716, -0.0037066147996727087)</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>(-0.00044048398486488656, -5.769911236564319e-06)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>(-0.00021090430295663343, 4.1233254404311016e-05)</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>(-8.13785410763523e-06, 2.7855216285062976e-05)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>(0.0006174590831356256, 0.0019669174992209496)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>(-0.0006029993732018713, -0.00017184188997214353)</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>(-8.296522091894037e-05, 8.456550605412343e-05)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>(0.0, 0.0)</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>(0.00030542506497996695, 0.0022948153721223485)</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>(0.0001625787219967029, 0.0007265949251628497)</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>(-0.00019536333650756893, -3.2063021052162015e-05)</t>
+        </is>
+      </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>(0.02126994414856681, 0.07087367579398138)</t>
+        </is>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>(-0.0016493022420456644, -7.388813922253328e-05)</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>(-7.373503938456802e-05, -3.182885519399301e-06)</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>(-0.002989873691417444, -0.0007341966876625232)</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>(-8.371755607819705e-05, 3.0078333327532997e-05)</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>(-0.00017403798565344714, 6.335306780686174e-05)</t>
+        </is>
+      </c>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>(0.0004414606922316211, 0.0013561747631702953)</t>
+        </is>
+      </c>
+      <c r="W7" t="inlineStr">
+        <is>
+          <t>(-0.001929358345626545, -0.000642668667454384)</t>
+        </is>
+      </c>
+      <c r="X7" t="inlineStr">
+        <is>
+          <t>(-0.0014704641028177219, -0.00032432520324388796)</t>
+        </is>
+      </c>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>(0.0006544385446804906, 0.001956711537100905)</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>(-0.00024037208997418233, -2.898391078272764e-06)</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>(-0.0006095324471212599, -3.6578157880316786e-05)</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>(3.476603088712148e-05, 0.00014515579996807147)</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>(4.313619662297329e-05, 0.00016905225295647613)</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>(-0.0004607189570341941, 4.8711193311980466e-05)</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
+          <t>(-0.003375881798028882, -0.0010239839895690521)</t>
+        </is>
+      </c>
+      <c r="AF7" t="inlineStr">
+        <is>
+          <t>(-0.0002543015776197495, -6.730521269868896e-05)</t>
+        </is>
+      </c>
+      <c r="AG7" t="inlineStr">
+        <is>
+          <t>(-0.000369862965430046, 5.7632690252000014e-05)</t>
+        </is>
+      </c>
+      <c r="AH7" t="inlineStr">
+        <is>
+          <t>(4.6145652124048514e-05, 0.0004260025234959059)</t>
+        </is>
+      </c>
+      <c r="AI7" t="inlineStr">
+        <is>
+          <t>(0.0002194148170348379, 0.0006026932474802826)</t>
+        </is>
+      </c>
+      <c r="AJ7" t="inlineStr">
+        <is>
+          <t>(-9.2882989198787e-06, 8.82118249217497e-05)</t>
+        </is>
+      </c>
+      <c r="AK7" t="inlineStr">
+        <is>
+          <t>(0.0003339732556027363, 0.0009779888375546642)</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update on context-specific model generation
</commit_message>
<xml_diff>
--- a/Data/ZeLa Data/specific_rates_R.xlsx
+++ b/Data/ZeLa Data/specific_rates_R.xlsx
@@ -8268,47 +8268,47 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>(0.006980490755421609, 0.011724525651933354)</t>
+          <t>(0.008166499479549545, 0.010538516927805419)</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(0.3054587191163002, 0.36768956628615557)</t>
+          <t>(0.321016430908764, 0.3521318544936917)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(0.03382876556351397, 0.03763290718946985)</t>
+          <t>(0.03477980097000294, 0.03668187178298088)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(0.008365335505423335, 0.024706182376133055)</t>
+          <t>(0.012450547223100766, 0.020620970658455626)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>(0.13533074143088733, 0.15587336717415232)</t>
+          <t>(0.14046639786670356, 0.15073771073833608)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(-0.03429380295821653, -0.005535191144234054)</t>
+          <t>(-0.027104150004720915, -0.012724844097729674)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>(-0.29168714341151875, -0.10165962153577811)</t>
+          <t>(-0.2441802629425836, -0.14916650200471326)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(0.010442903455503586, 0.055499169136505225)</t>
+          <t>(0.021706969875753997, 0.04423510271625481)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>(0.010926764882662946, 0.011491061728186832)</t>
+          <t>(0.011067839094043918, 0.011349987516805861)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -8318,17 +8318,17 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>(-0.016592725860987312, -0.005034366195191302)</t>
+          <t>(-0.01370313594453831, -0.007923956111640304)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>(0.0029006278169949953, 0.10899483341178243)</t>
+          <t>(0.029424179215691855, 0.08247128201308557)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>(0.07692077840289853, 0.09640683472389681)</t>
+          <t>(0.08179229248314811, 0.09153532064364724)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -8338,37 +8338,37 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>(-1.6786273279256634, 0.911950170768091)</t>
+          <t>(-1.0309829532522248, 0.2643057960946525)</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>(-0.00434533053545956, 0.05349828220988641)</t>
+          <t>(0.010115572650876932, 0.039037379023549916)</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>(-0.6782472745614954, -0.41556286165956086)</t>
+          <t>(-0.6125761713360117, -0.48123396488504444)</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>(0.02341516305267049, 0.032031273734593316)</t>
+          <t>(0.025569190723151194, 0.02987724606411261)</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>(-0.015611503012663036, 0.0034068197420656686)</t>
+          <t>(-0.01085692232398086, -0.0013477609466165073)</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>(-0.012588236475553143, -0.0009479448786626349)</t>
+          <t>(-0.009678163576330516, -0.003858017777885262)</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>(-0.025853996100852313, -0.007732345411183863)</t>
+          <t>(-0.0213235834284352, -0.012262758083600975)</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -8378,17 +8378,17 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>(1.4273446116071347, 1.7935010646873695)</t>
+          <t>(1.5188837248771934, 1.7019619514173108)</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>(-0.04198330335835026, -0.015693134207211114)</t>
+          <t>(-0.035410761070565476, -0.0222656764949959)</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>(-0.052161543186050645, -0.0031887940662676667)</t>
+          <t>(-0.0399183559061049, -0.015431981346213411)</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -8398,52 +8398,52 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>(-0.01516817696302043, -0.007961603225463555)</t>
+          <t>(-0.01336653352863121, -0.009763246659852775)</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>(-0.010731933987393777, 0.012534001704794191)</t>
+          <t>(-0.004915450064346785, 0.006717517781747199)</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>(0.023005412685814075, 0.16054961308617646)</t>
+          <t>(0.05739146278590467, 0.12616356298608586)</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>(0.2110402511714216, 0.30977491115612604)</t>
+          <t>(0.23572391616759772, 0.2850912461599499)</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>(-0.08724621411093643, -0.053020435974206706)</t>
+          <t>(-0.078689769576754, -0.06157688050838914)</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>(-0.21629087325901078, -0.053334840858248495)</t>
+          <t>(-0.1755518651588202, -0.09407384895843907)</t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>(-0.03584681090475491, 0.0022372500117713023)</t>
+          <t>(-0.026325795675623355, -0.007283765217360251)</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>(-0.011701558097023921, -0.003544112267049048)</t>
+          <t>(-0.009662196639530203, -0.005583473724542766)</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>(0.005445106527599144, 0.015180685499380401)</t>
+          <t>(0.007879001270544458, 0.012746790756435086)</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>(-0.03472606790802207, -0.01349770032415601)</t>
+          <t>(-0.02941897601205555, -0.018804792220122525)</t>
         </is>
       </c>
     </row>
@@ -8455,32 +8455,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(-0.00014873598323341864, 0.0001103894966851675)</t>
+          <t>(-8.39546132537721e-05, 4.560812670552097e-05)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(-0.001301647914955597, 0.0017121380702289505)</t>
+          <t>(-0.0005482014186594601, 0.0009586915739328136)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(-0.013105665505329097, 0.009147305667877467)</t>
+          <t>(-0.007542422712027455, 0.0035840628745758265)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(-0.020118031704357525, 0.015582819577074065)</t>
+          <t>(-0.011192818883999629, 0.006657606756716167)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>(-0.0024756529728442293, 0.001072149347114183)</t>
+          <t>(-0.0015887023928546262, 0.00018519876712457992)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>(-0.0003816106700790472, 0.0002739918171888285)</t>
+          <t>(-0.0002177100482620783, 0.00011009119537185955)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -8490,17 +8490,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(-0.00048625530215011656, 0.0007671597526458974)</t>
+          <t>(-0.0001729015384511131, 0.00045380598894689394)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>(-3.5231391038659585e-05, 5.711434319280575e-05)</t>
+          <t>(-1.2144957480793252e-05, 3.402790963493942e-05)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>(-0.0003071259173835132, 0.0005373012558524253)</t>
+          <t>(-9.601912407452855e-05, 0.0003261944625434407)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -8510,127 +8510,127 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>(-0.0019742131984348647, 0.0031981692320309785)</t>
+          <t>(-0.0006811175908184038, 0.0019050736244145177)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>(-0.000785485289232253, 0.0012917878293231657)</t>
+          <t>(-0.0002661670095933984, 0.0007724695496843109)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>(-0.0002424853467108129, 0.00014048389952536322)</t>
+          <t>(-0.00014674303515176888, 4.474158796631919e-05)</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>(-0.038378254122169685, 0.05758471746600675)</t>
+          <t>(-0.014387511225125578, 0.03359397456896264)</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>(-0.0001520417572878674, 0.00018349445054975292)</t>
+          <t>(-6.815770532846231e-05, 9.961039859034785e-05)</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>(-5.568945604474948e-05, 2.462024101282121e-05)</t>
+          <t>(-3.5612031780356806e-05, 4.542816748428538e-06)</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>(-0.0020672599628087374, 0.0016311820060914168)</t>
+          <t>(-0.001142649470583699, 0.0007065715138663782)</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>(-7.038887736005587e-05, 6.517904164622985e-05)</t>
+          <t>(-3.649689760848444e-05, 3.128706189465842e-05)</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>(-0.0009035416348096244, 0.0007137594476462589)</t>
+          <t>(-0.0004992163641956536, 0.00030943417703228806)</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>(-1.3342991739731411e-05, 3.3272877481408806e-05)</t>
+          <t>(-1.6890244344463573e-06, 2.161891017612375e-05)</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>(-2.5134586211812084e-05, 8.784962106535719e-05)</t>
+          <t>(3.111465607480232e-06, 5.960356924606487e-05)</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>(-0.039668397725792726, 0.026269893383163035)</t>
+          <t>(-0.023183824948553783, 0.009785320605924096)</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>(-0.00013663705946738224, 0.00010791320494328895)</t>
+          <t>(-7.549949336471446e-05, 4.677563884062115e-05)</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>(-0.00027366522691634507, 0.00027698163767189655)</t>
+          <t>(-0.00013600351076928463, 0.00013931992152483617)</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>(-0.0004167366085000001, 0.0002523940332481244)</t>
+          <t>(-0.00024945394806296896, 8.511137281109325e-05)</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>(-0.00015422711072343807, 0.00011110052463746553)</t>
+          <t>(-8.789520188321216e-05, 4.476861579723963e-05)</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>(-8.99017862861481e-06, 1.7821660526158052e-05)</t>
+          <t>(-2.287218839921593e-06, 1.1118700737464837e-05)</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>(-0.0008769019927273964, 0.0007126058642462976)</t>
+          <t>(-0.00047952502848397284, 0.00031522890000287417)</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>(-0.00045999897520302894, 0.0013709765693132655)</t>
+          <t>(-2.2550890739553493e-06, 0.0009132326831841919)</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>(-0.0008371691036118944, 0.000404401727909164)</t>
+          <t>(-0.0005267763957316298, 9.40090200288994e-05)</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>(-0.00032196528773957095, 0.00016861802738020356)</t>
+          <t>(-0.0001993194589596273, 4.597219860025995e-05)</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>(-0.0003918514772094398, 0.00030463719194550345)</t>
+          <t>(-0.00021772930992070398, 0.00013051502465676764)</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>(-2.121032403814515e-05, 1.5104536189068671e-05)</t>
+          <t>(-1.2131608981341694e-05, 6.025821132265216e-06)</t>
         </is>
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>(-4.112205571563613e-05, 5.609829684740075e-05)</t>
+          <t>(-1.681696757487691e-05, 3.179320870664153e-05)</t>
         </is>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>(8.917378665226131e-06, 4.24851531480716e-05)</t>
+          <t>(1.73093222859375e-05, 3.409320952736023e-05)</t>
         </is>
       </c>
     </row>
@@ -8642,127 +8642,127 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(0.002434203694290207, 0.004562976907096232)</t>
+          <t>(0.0029663969974917134, 0.0040307836038947255)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(0.07279641307248068, 0.12186930266457079)</t>
+          <t>(0.0850646354705032, 0.10960108026654826)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(0.031020192288701405, 0.03747941279190218)</t>
+          <t>(0.0326349974145016, 0.035864607666101986)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(0.0007901936812916199, 0.0016317672211287472)</t>
+          <t>(0.0010005870662509017, 0.0014213738361694653)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(0.03983662033636283, 0.05705449498476117)</t>
+          <t>(0.04414108899846242, 0.05275002632266158)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(-0.019935448577103103, -0.011761487400016937)</t>
+          <t>(-0.017891958282831563, -0.013804977694288479)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(-0.11003635045489456, -0.07907240256893582)</t>
+          <t>(-0.10229536348340487, -0.0868133895404255)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(0.010442982014861726, 0.022420803064034316)</t>
+          <t>(0.013437437277154874, 0.01942634780174117)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(0.0008191393700247571, 0.0017593610751020447)</t>
+          <t>(0.001054194796294079, 0.001524305648832723)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(0.004712241827476959, 0.007823500580973999)</t>
+          <t>(0.0054900565158512195, 0.007045685892599738)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>(-0.0037764144059367765, -0.0027439842541121186)</t>
+          <t>(-0.003518306867980612, -0.003002091792068283)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>(-0.011572613338819787, 0.0947514727395521)</t>
+          <t>(0.015008408180773185, 0.06817045121995913)</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>(0.023189840087647486, 0.03115571194073608)</t>
+          <t>(0.025181308050919633, 0.029164243977463932)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>(-0.0005146181996300925, 0.0009323105516569979)</t>
+          <t>(-0.00015288601180831992, 0.0005705783638352253)</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>(-0.6040237929583947, -0.39853389023760394)</t>
+          <t>(-0.5526513172781969, -0.44990636591780164)</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>(0.006542882443800259, 0.017375799270177683)</t>
+          <t>(0.009251111650394616, 0.014667570063583327)</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>(-0.10889761383180706, -0.09233662508435016)</t>
+          <t>(-0.10475736664494283, -0.09647687227121439)</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>(0.008744977987028368, 0.01633699396750253)</t>
+          <t>(0.010642981982146908, 0.014438989972383989)</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>(-0.006887880870123379, -0.004949643011631271)</t>
+          <t>(-0.006403321405500352, -0.005434202476254297)</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>(-0.00542963151692638, 0.0009834426653616366)</t>
+          <t>(-0.003826362971354376, -0.0006198258802103675)</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>(-0.016687369642772808, -0.0106161442320302)</t>
+          <t>(-0.015169563290087156, -0.012133950584715853)</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>(-0.0003799091500511334, 0.0014166433354745006)</t>
+          <t>(6.922897133027506e-05, 0.000967505214093092)</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
         <is>
-          <t>(0.6230202700967561, 0.7939250058598758)</t>
+          <t>(0.665746454037536, 0.7511988219190959)</t>
         </is>
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>(-0.026726233036018725, -0.01848083396090467)</t>
+          <t>(-0.02466488326724021, -0.020542183729683184)</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>(-0.027683229262136774, -0.017483238321922882)</t>
+          <t>(-0.025133231527083303, -0.020033236056976354)</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
@@ -8772,52 +8772,52 @@
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>(-0.008223778093504571, -0.006383941081620491)</t>
+          <t>(-0.007763818840533552, -0.006843900334591512)</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>(-0.009988503609417844, -0.00768030163863205)</t>
+          <t>(-0.009411453116721395, -0.008257352131328497)</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>(-0.04531407621252179, -0.023698947036880674)</t>
+          <t>(-0.03991029391861151, -0.02910272933079095)</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>(-0.00037608955576437855, 0.019676563020515535)</t>
+          <t>(0.0046370735883056, 0.014663399876445556)</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>(0.0009793777080232698, 0.006055779449504891)</t>
+          <t>(0.002248478143393675, 0.0047866790141344855)</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>(-0.06700522929642376, -0.04565843556076462)</t>
+          <t>(-0.06166853086250897, -0.0509951339946794)</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>(-0.031173475384535992, -0.004074509165846925)</t>
+          <t>(-0.024398733829863725, -0.01084925072051919)</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>(-0.004027350686137971, -0.002531077188728636)</t>
+          <t>(-0.0036532823117856376, -0.00290514556308097)</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>(-0.011355096709556294, -0.009219634081694628)</t>
+          <t>(-0.010821231052590877, -0.009753499738660045)</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>(-0.02110366872164228, -0.01631627209808975)</t>
+          <t>(-0.019906819565754148, -0.017513121253977883)</t>
         </is>
       </c>
     </row>
@@ -8829,127 +8829,127 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(0.00028280639128655484, 0.0004890858789320631)</t>
+          <t>(0.00033437626319793187, 0.00043751600702068605)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(-0.005725504506143511, -0.0007968842592079757)</t>
+          <t>(-0.004493349444409627, -0.0020290393209418597)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(0.0146336547171366, 0.019135784019938994)</t>
+          <t>(0.015759187042837196, 0.018010251694238397)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(0.004429178142518867, 0.00794487056707895)</t>
+          <t>(0.005308101248658888, 0.007065947460938929)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>(0.0003862475471303698, 0.006541298474616925)</t>
+          <t>(0.0019250102790020086, 0.005002535742745286)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>(-0.00436468445562047, -0.00277936589014081)</t>
+          <t>(-0.003968354814250555, -0.003175695531510725)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>(-0.019393682514807248, -0.010031055009814552)</t>
+          <t>(-0.017053025638559073, -0.012371711886062725)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(-0.0017538268514956106, -0.001197817680677546)</t>
+          <t>(-0.0016148245587910943, -0.0013368199733820622)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>(0.000943119361521074, 0.0011464867077687975)</t>
+          <t>(0.0009939611980830049, 0.0010956448712068666)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>(0.001986036366486741, 0.0026168631751864405)</t>
+          <t>(0.0021437430686616662, 0.0024591564730115155)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>(-0.00039954726366306885, -0.0002451061094765542)</t>
+          <t>(-0.0003609369751164402, -0.00028371639802318287)</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>(-0.031140684877408988, 0.035443314181312253)</t>
+          <t>(-0.014494685112728679, 0.018797314416631943)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>(0.006733634747037004, 0.009657048735276678)</t>
+          <t>(0.007464488244096922, 0.00892619523821676)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>(-0.00019166779043844275, 0.00019523163629357146)</t>
+          <t>(-9.494293375543921e-05, 9.85067796105679e-05)</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>(-0.18355723802214335, -0.059829374402763875)</t>
+          <t>(-0.15262527211729848, -0.09076134030760874)</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>(-0.00013484151021487091, 0.0022428448258565614)</t>
+          <t>(0.0004595800738029872, 0.0016484232418387033)</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>(-0.006215204627712164, -0.0031635017224734933)</t>
+          <t>(-0.0054522789014024966, -0.0039264274487831605)</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>(0.003907070428407259, 0.006155326045495116)</t>
+          <t>(0.004469134332679223, 0.005593262141223152)</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>(-0.0017043421609033052, -0.001354638632664341)</t>
+          <t>(-0.0016169162788435643, -0.001442064514724082)</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>(-0.0013768213063086244, 0.00025478465503170756)</t>
+          <t>(-0.0009689198159735414, -0.00015311683530337542)</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>(-0.0053607288044757884, -0.0029183208451135385)</t>
+          <t>(-0.004750126814635226, -0.003528922834954101)</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>(0.0007859251133422251, 0.0009556805222305334)</t>
+          <t>(0.0008283639655643022, 0.0009132416700084563)</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>(0.035035967517283724, 0.10938616284778202)</t>
+          <t>(0.05362351634990829, 0.09079861401515744)</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>(-0.008403597075256482, -0.00458098005609439)</t>
+          <t>(-0.007447942820465959, -0.005536634310884913)</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>(-0.005984423640692276, -0.0034864037317761977)</t>
+          <t>(-0.0053599186634632565, -0.004110908709005217)</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
@@ -8959,52 +8959,52 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>(-0.0019704675728161336, -0.0012500946880935)</t>
+          <t>(-0.0017903743516354753, -0.0014301879092741582)</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>(-0.0032936162906066924, -0.0016936503257545374)</t>
+          <t>(-0.0028936247993936537, -0.0020936418169675763)</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>(-0.0063970793230042275, -0.0035086726913778187)</t>
+          <t>(-0.005674977665097626, -0.0042307743492844205)</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>(-0.0010661673730184627, 0.0029170260668264967)</t>
+          <t>(-7.036901305722287e-05, 0.0019212277068652568)</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>(-0.005776431337127363, -0.003335200826784368)</t>
+          <t>(-0.005166123709541615, -0.0039455084543701165)</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>(-0.01927355383196927, -0.012105401604668359)</t>
+          <t>(-0.017481515775144042, -0.013897439661493587)</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>(-0.006174798456691853, -0.0015269565614003749)</t>
+          <t>(-0.005012837982868983, -0.0026889170352232443)</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>(-0.0014509579738269612, -0.0010874211015393066)</t>
+          <t>(-0.0013600737557550476, -0.0011783053196112202)</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>(-0.0017169870868334568, -0.0012322561791181658)</t>
+          <t>(-0.001595804359904634, -0.0013534389060469885)</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>(-0.006132445595825549, -0.003453566603434641)</t>
+          <t>(-0.005462725847727822, -0.004123286351532368)</t>
         </is>
       </c>
     </row>
@@ -9016,127 +9016,127 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(-0.00012899630340514471, 6.804095832712931e-05)</t>
+          <t>(-7.973698797207622e-05, 1.8781642894060807e-05)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(-0.0017234912393393677, 0.00018615713437206008)</t>
+          <t>(-0.0012460791459115107, -0.00029125495905579687)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(-0.0036761260349289547, 2.44921589494958e-05)</t>
+          <t>(-0.002750971486459342, -0.0009006623895201169)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(-0.005248070742966578, 0.00028489295809003496)</t>
+          <t>(-0.003864829817702425, -0.0010983479671741183)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>(-0.0003087130899605918, 0.0020152364744208994)</t>
+          <t>(0.00027227430113478104, 0.0014342490833255267)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>(-2.3720873366897096e-05, 0.00024233525905622644)</t>
+          <t>(4.279315973888379e-05, 0.00017582122595044558)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>(5.029507886481605e-07, 0.0008016537093478871)</t>
+          <t>(0.0002007906404284579, 0.0006013660197080774)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(-9.778201432733097e-06, 0.0004880626212511428)</t>
+          <t>(0.00011468200423823589, 0.0003636024155801739)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>(-0.0002179135006468962, -5.269081203294502e-06)</t>
+          <t>(-0.00016475239578599577, -5.843018606419492e-05)</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>(-0.00024763627758070535, -1.0597197450107622e-05)</t>
+          <t>(-0.00018837650754805594, -6.985696748275705e-05)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>(-1.567857013689985e-07, 2.9121060649262476e-05)</t>
+          <t>(7.16267588628887e-06, 2.1801599061604607e-05)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>(-0.0019543910070405662, 0.0024590088249430626)</t>
+          <t>(-0.0008510410490446591, 0.0013556588669471552)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>(-0.00021427975806705292, 1.854023857053485e-05)</t>
+          <t>(-0.00015607475890765598, -3.966476058886209e-05)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>(-1.6811960879773974e-05, -7.0213372705377015e-06)</t>
+          <t>(-1.4364304977464906e-05, -9.468993172846771e-06)</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>(-0.007595402240404428, 0.034122886338510384)</t>
+          <t>(0.0028341699043242744, 0.023693314193781678)</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>(-0.0001128483772276786, 0.00016064300857757688)</t>
+          <t>(-4.447553077636474e-05, 9.2270162126263e-05)</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>(-1.4698913511998324e-05, 8.113528689146464e-06)</t>
+          <t>(-8.995802961712128e-06, 2.4104181388602668e-06)</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>(-0.0003873239255164395, 0.00011980810794137039)</t>
+          <t>(-0.00026054091715198703, -6.974900423082074e-06)</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>(-4.578397057199321e-05, 0.0001513538001357662)</t>
+          <t>(3.500472104946645e-06, 0.00010206935745882636)</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>(-5.4786048223963383e-05, 2.1722980346586797e-05)</t>
+          <t>(-3.5658791081325836e-05, 2.595723203949253e-06)</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>(-1.4805190992828654e-05, 0.00038403443966886805)</t>
+          <t>(8.490471667259552e-05, 0.00028432453200344387)</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>(-0.0002893002185483923, -4.3800881630786856e-05)</t>
+          <t>(-0.00022792538431899094, -0.00010517571586018822)</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>(-0.026482498825595144, 0.01349910294055023)</t>
+          <t>(-0.0164870983840588, 0.0035037024990138875)</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>(6.799988740501732e-06, 0.0006260280822968809)</t>
+          <t>(0.00016160701212959653, 0.00047122105890778617)</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>(2.229839596837893e-05, 0.0002741910562264485)</t>
+          <t>(8.527156103289632e-05, 0.0002112178911619311)</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
@@ -9146,52 +9146,52 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>(-9.278020935745977e-06, 0.00014115960461807454)</t>
+          <t>(2.833138545270915e-05, 0.0001035501982296194)</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>(3.582177376998947e-06, 0.00017434419811683912)</t>
+          <t>(4.6272682561958993e-05, 0.00013165369293187908)</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>(-8.483391213009322e-05, 0.00039606211699773)</t>
+          <t>(3.5390095151862584e-05, 0.0002758381097157742)</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>(-0.00022279203343288827, 1.4182134625809396e-05)</t>
+          <t>(-0.00016354849141821386, -4.506140738886502e-05)</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>(-6.558710131877239e-06, 0.00013408375766381543)</t>
+          <t>(2.8601906817045925e-05, 9.892314071489225e-05)</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>(-1.0316224628850637e-05, 0.0008875511793867718)</t>
+          <t>(0.000214150626375055, 0.0006630843283828662)</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>(-5.961787397352869e-05, 0.00015492490382007013)</t>
+          <t>(-5.98217952512898e-06, 0.00010128920937167043)</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>(-2.733051156084094e-05, 0.0002092739367388581)</t>
+          <t>(3.182060051408382e-05, 0.00015012282466393334)</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>(-2.7408672629630304e-05, 0.00019698513980188494)</t>
+          <t>(2.8689780478248507e-05, 0.00014088668669400613)</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>(3.587661341555729e-07, 0.0003814721776299158)</t>
+          <t>(9.563711900809563e-05, 0.00028619382475597577)</t>
         </is>
       </c>
     </row>
@@ -9203,52 +9203,52 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(-0.0007017172287941157, -0.00031180729031089175)</t>
+          <t>(-0.0006042397441733097, -0.00040928477493169774)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(-0.009924642196731155, 0.014102118098609931)</t>
+          <t>(-0.003917952122895883, 0.00809542802477466)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(-0.01632998479943893, -0.0006596675553291863)</t>
+          <t>(-0.012412405488411493, -0.004577246866356622)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(-0.05983168837494649, -0.010288843495956136)</t>
+          <t>(-0.0474459771551989, -0.022674554715703725)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>(-0.01787435690354429, 0.009773974422634148)</t>
+          <t>(-0.01096227407199968, 0.0028618915910895385)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>(-5.551760462423446e-05, 0.0005356316071693222)</t>
+          <t>(9.226969832415468e-05, 0.000387844304220933)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>(-3.5569354927646936e-05, 0.00011971764062881488)</t>
+          <t>(3.2523939614685185e-06, 8.089589173969943e-05)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(-0.0007944241890876485, 0.00691083303737919)</t>
+          <t>(0.0011318901175290611, 0.00498451873076248)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>(-0.0009909068218576012, 4.7633288674584775e-05)</t>
+          <t>(-0.0007312717942245547, -0.00021200173895846171)</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>(9.430319302333322e-06, 0.0013761779823309858)</t>
+          <t>(0.0003511172350594964, 0.0010344910665738226)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -9258,127 +9258,127 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>(-0.0013237381700689367, 0.004554738240347053)</t>
+          <t>(0.00014588093253506081, 0.0030851191377430556)</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>(-0.0016451989424496765, 0.006358955899859008)</t>
+          <t>(0.0003558397681274945, 0.004357917189281836)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>(-0.0013515443171293906, 0.0002472252066486731)</t>
+          <t>(-0.0009518519361848747, -0.00015246717429584283)</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>(-0.0345602431335538, 0.2960902663301651)</t>
+          <t>(0.04810238423237592, 0.21342763896423536)</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>(-0.004841753230222747, 0.00243020780500051)</t>
+          <t>(-0.0030237629714169323, 0.000612217546194696)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>(-0.00022192797074143265, 7.749046832070919e-06)</t>
+          <t>(-0.00016450871634805675, -4.967020756130497e-05)</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>(-0.005511517969111006, 0.0021161272129662364)</t>
+          <t>(-0.0036046066735916957, 0.00020921591744692573)</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>(-3.246632177545003e-05, 0.00013251162598672592)</t>
+          <t>(8.77816516509396e-06, 9.126713904618195e-05)</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>(-0.00027876708548495253, 0.0005608501277978336)</t>
+          <t>(-6.886278216425602e-05, 0.00035094582447713703)</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>(-0.0009345761191557909, 0.002719018767226939)</t>
+          <t>(-2.1177397560108468e-05, 0.0018056200456312566)</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>(-0.003085992226273302, 0.0014346838432547243)</t>
+          <t>(-0.001955823208891295, 0.00030451482587271785)</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>(-0.11591598533113212, -0.07786450938252146)</t>
+          <t>(-0.10640311634397945, -0.08737737836967413)</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>(-0.0014914085679053543, 0.0037104642407810333)</t>
+          <t>(-0.00019094036573375742, 0.002409996038609436)</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>(-0.00025417378613694597, 0.0006965416765438335)</t>
+          <t>(-1.6494920466751114e-05, 0.0004588628108736386)</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>(-0.004272587722256135, 0.000867296324421354)</t>
+          <t>(-0.0029876167105867624, -0.0004176746872480181)</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>(2.5572724611364447e-05, 0.0003298215407605105)</t>
+          <t>(0.00010163492864865095, 0.00025375933672322395)</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>(1.4321780179364933e-05, 0.0006666411496511926)</t>
+          <t>(0.00017740162254732184, 0.0005035613072832357)</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>(-4.044378074925109e-05, 0.0014412028139349213)</t>
+          <t>(0.000329967867921792, 0.0010707911652638783)</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>(-0.006279252934961655, 0.002740563941370182)</t>
+          <t>(-0.004024298715878696, 0.0004856097222872228)</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>(-0.0016721496382802606, 0.0004163866251146695)</t>
+          <t>(-0.0011500155724315283, -0.00010574744073406307)</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>(-0.0010015798107148696, 0.0005819039334489078)</t>
+          <t>(-0.0006057088746739254, 0.00018603299740796344)</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>(-0.001946903916067561, 0.0018857778728757998)</t>
+          <t>(-0.0009887334688317207, 0.0009276074256399597)</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>(0.0002653265245707283, 0.0007873873250375595)</t>
+          <t>(0.0003958417246874361, 0.0006568721249208517)</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>(-0.00011504492088218235, 4.99530901424839e-05)</t>
+          <t>(-7.379541812601579e-05, 8.703587386317335e-06)</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>(-0.0007463659919571643, 0.002103585669771429)</t>
+          <t>(-3.387807652501602e-05, 0.0013910977543392807)</t>
         </is>
       </c>
     </row>
@@ -9601,42 +9601,42 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>(0.2843722527201595, 0.43256814512792024)</t>
+          <t>(0.32142122582209964, 0.3955191720259801)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>(0.0304758062687544, 0.040174165467906524)</t>
+          <t>(0.03290039606854243, 0.03774957566811849)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>(0.02019954219212499, 0.033951428885071785)</t>
+          <t>(0.023637513865361687, 0.03051345721183509)</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>(0.1220582558482064, 0.21594382265092615)</t>
+          <t>(0.14552964754888634, 0.19247243095024621)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>(-0.042087333321744295, -0.00481579006747309)</t>
+          <t>(-0.032769447508176494, -0.014133675881040891)</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>(-0.3939606076008609, -0.1928429069623105)</t>
+          <t>(-0.3436811824412233, -0.2431223321219481)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(0.004021199888929097, 0.053419665222494986)</t>
+          <t>(0.016370816222320568, 0.04107004888910351)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>(0.0030881279589110256, 0.01592926115391485)</t>
+          <t>(0.006298411257661982, 0.012718977855163894)</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -9646,17 +9646,17 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>(-0.016228154785355407, -0.010820169660146912)</t>
+          <t>(-0.014876158504053286, -0.012172165941449035)</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>(-0.4357765577760694, 1.3284860252364594)</t>
+          <t>(0.005289087977062845, 0.8874203794833273)</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>(0.08843636352976685, 0.12556421702965578)</t>
+          <t>(0.09771832690473908, 0.11628225365468356)</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -9666,37 +9666,37 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>(-0.46063219257513033, 0.30556514971112003)</t>
+          <t>(-0.26908285700356777, 0.11401581413955741)</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>(-0.007617931381840328, 0.04682071023556142)</t>
+          <t>(0.005991729022510108, 0.03321104983121098)</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>(-0.6729556751459599, -0.36530776477992954)</t>
+          <t>(-0.5960436975544523, -0.44221974237143713)</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
         <is>
-          <t>(0.027745005834789775, 0.04964438639249436)</t>
+          <t>(0.033219850974215925, 0.04416954125306821)</t>
         </is>
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>(-0.02416641589907178, 0.0018067164056212188)</t>
+          <t>(-0.017673132822898528, -0.00468656667055203)</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
         <is>
-          <t>(-0.030190140253075953, 0.012156684321093507)</t>
+          <t>(-0.019603434109533587, 0.0015699781775511418)</t>
         </is>
       </c>
       <c r="V2" t="inlineStr">
         <is>
-          <t>(-0.054652608545042045, 0.007882092238180757)</t>
+          <t>(-0.03901893334923635, -0.0077515829576249445)</t>
         </is>
       </c>
       <c r="W2" t="inlineStr">
@@ -9711,12 +9711,12 @@
       </c>
       <c r="Y2" t="inlineStr">
         <is>
-          <t>(-0.08237632422535054, 0.006011656538394132)</t>
+          <t>(-0.06027932903441437, -0.016085338652542035)</t>
         </is>
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>(-0.051239191973542375, -0.009459837560270981)</t>
+          <t>(-0.04079435337022452, -0.01990467616358883)</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -9726,52 +9726,52 @@
       </c>
       <c r="AB2" t="inlineStr">
         <is>
-          <t>(-0.02666949859149547, -0.006471732547852799)</t>
+          <t>(-0.0216200570805848, -0.011521174058763467)</t>
         </is>
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>(-0.021376984275043667, 0.016986090073085058)</t>
+          <t>(-0.011786215688011484, 0.0073953214860528775)</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr">
         <is>
-          <t>(-0.06735686192217899, 0.21290687222577026)</t>
+          <t>(0.0027090716148083227, 0.14284093868878295)</t>
         </is>
       </c>
       <c r="AE2" t="inlineStr">
         <is>
-          <t>(0.18521037808707447, 0.3786828864665582)</t>
+          <t>(0.2335785051819454, 0.33031475937168725)</t>
         </is>
       </c>
       <c r="AF2" t="inlineStr">
         <is>
-          <t>(0.030840865081294445, 0.11838304434556521)</t>
+          <t>(0.05272640989736213, 0.09649749952949752)</t>
         </is>
       </c>
       <c r="AG2" t="inlineStr">
         <is>
-          <t>(-0.2585819184410899, -0.08973441892713044)</t>
+          <t>(-0.21637004356260006, -0.1319462938056203)</t>
         </is>
       </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>(-0.06331084851030629, -0.006204726056264431)</t>
+          <t>(-0.049034317896795826, -0.020481256669774895)</t>
         </is>
       </c>
       <c r="AI2" t="inlineStr">
         <is>
-          <t>(-0.010295790175785306, -0.0013592398007103712)</t>
+          <t>(-0.008061652582016573, -0.003593377394479105)</t>
         </is>
       </c>
       <c r="AJ2" t="inlineStr">
         <is>
-          <t>(-0.029905125325671217, 0.014272889087102792)</t>
+          <t>(-0.018860621722477718, 0.0032283854839092897)</t>
         </is>
       </c>
       <c r="AK2" t="inlineStr">
         <is>
-          <t>(-0.05818264213053942, -0.00023532294802524126)</t>
+          <t>(-0.04369581233491087, -0.014722152743653785)</t>
         </is>
       </c>
     </row>
@@ -9783,32 +9783,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>(-1.4515368576345884e-05, 1.7463223307122375e-05)</t>
+          <t>(-6.520720605478819e-06, 9.468575336255312e-06)</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>(-0.0017391347235528832, 0.001269893651068494)</t>
+          <t>(-0.0009868776298975388, 0.0005176365574131498)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>(-0.018243029392477503, 0.014480309648011986)</t>
+          <t>(-0.010062194632355132, 0.006299474887889614)</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>(-0.017893469015360753, 0.013505658744396487)</t>
+          <t>(-0.010043687075421444, 0.005655876804457177)</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>(-0.00024984046616538215, 0.00017125853596909135)</t>
+          <t>(-0.0001445657156317638, 6.598378543547296e-05)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>(-0.0003852276398486946, 0.0003038291021744218)</t>
+          <t>(-0.00021296345434291554, 0.00013156491666864266)</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -9818,17 +9818,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(-0.00029288600714901084, 0.0002507544227418563)</t>
+          <t>(-0.00015697589967629406, 0.0001148443152691395)</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>(-0.0002377262371558444, 0.00018915383449683086)</t>
+          <t>(-0.00013100621924267558, 8.243381658366205e-05)</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>(-0.000323013139196167, 0.0002465878084097258)</t>
+          <t>(-0.0001806129022946938, 0.00010418757150825263)</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -9838,127 +9838,127 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>(-0.0004637198794008105, 0.0009039421799310139)</t>
+          <t>(-0.00012180436456785441, 0.0005620266650980578)</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>(-0.0005601354275838037, 0.0006193975534331748)</t>
+          <t>(-0.00026525218232955906, 0.00032451430817893016)</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>(-4.037908312716791e-05, 2.7630262139519176e-05)</t>
+          <t>(-2.3376746810496142e-05, 1.0627925822847402e-05)</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>(-0.038652352763228884, 0.04572492308583144)</t>
+          <t>(-0.0175580338009638, 0.024630604123566362)</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>(-0.0015021370433588224, 0.0011346330199244379)</t>
+          <t>(-0.0008429445275380072, 0.00047544050410362293)</t>
         </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>(-0.00012078684564050104, 8.291659324724066e-05)</t>
+          <t>(-6.986098591856563e-05, 3.1990733525305225e-05)</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
         <is>
-          <t>(-0.0028067941318696177, 0.002099279358038573)</t>
+          <t>(-0.00158027575939257, 0.0008727609855615255)</t>
         </is>
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>(-0.00014957876760806363, 9.74033477928648e-05)</t>
+          <t>(-8.783323875783154e-05, 3.565781894263268e-05)</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t>(-0.0006256826535268929, 0.0004331355965461098)</t>
+          <t>(-0.0003609780910086422, 0.0001684310340278591)</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
         <is>
-          <t>(-0.00040685993804784885, 0.0004802869359522899)</t>
+          <t>(-0.00018507321954781413, 0.00025850021745225525)</t>
         </is>
       </c>
       <c r="W3" t="inlineStr">
         <is>
-          <t>(-0.001383401452052828, 0.000992472761288315)</t>
+          <t>(-0.0007894328987175423, 0.0003985042079530292)</t>
         </is>
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>(-0.0005253321004711686, 0.0004284865234525724)</t>
+          <t>(-0.00028687744449023335, 0.00019003186747163718)</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">
         <is>
-          <t>(-0.0004988344091285105, 0.0006654872334412008)</t>
+          <t>(-0.0002077539984860827, 0.00037440682279877294)</t>
         </is>
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>(-0.00022930820281351965, 0.00021987568147558488)</t>
+          <t>(-0.00011701223174124352, 0.00010757971040330875)</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>(-0.0011409439219904325, 0.0007572166566540523)</t>
+          <t>(-0.0006664037773293114, 0.00028267651199293106)</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">
         <is>
-          <t>(-1.9607042149316058e-05, 3.519979087892484e-05)</t>
+          <t>(-5.905333892255831e-06, 2.149808262186462e-05)</t>
         </is>
       </c>
       <c r="AC3" t="inlineStr">
         <is>
-          <t>(-0.00011676951414001453, 8.252258378079587e-05)</t>
+          <t>(-6.694648965981193e-05, 3.269955930059327e-05)</t>
         </is>
       </c>
       <c r="AD3" t="inlineStr">
         <is>
-          <t>(-9.380854291141933e-05, 0.00015598748007260857)</t>
+          <t>(-3.135953716541235e-05, 9.353847432660161e-05)</t>
         </is>
       </c>
       <c r="AE3" t="inlineStr">
         <is>
-          <t>(-0.005915699353520566, 0.004374492111881254)</t>
+          <t>(-0.0033431514871701106, 0.0018019442455307992)</t>
         </is>
       </c>
       <c r="AF3" t="inlineStr">
         <is>
-          <t>(-0.00021515234203605562, 0.00041168231658209704)</t>
+          <t>(-5.844367738151745e-05, 0.0002549736519275589)</t>
         </is>
       </c>
       <c r="AG3" t="inlineStr">
         <is>
-          <t>(-0.0004408900521677706, 0.0003182731358294892)</t>
+          <t>(-0.00025109925516845566, 0.00012848233883017425)</t>
         </is>
       </c>
       <c r="AH3" t="inlineStr">
         <is>
-          <t>(-0.0011850301146972028, 0.000870015865672336)</t>
+          <t>(-0.000671268619604818, 0.00035625437057995135)</t>
         </is>
       </c>
       <c r="AI3" t="inlineStr">
         <is>
-          <t>(-0.0001830938485120243, 0.0002446339547829472)</t>
+          <t>(-7.616189768828141e-05, 0.00013770200395920435)</t>
         </is>
       </c>
       <c r="AJ3" t="inlineStr">
         <is>
-          <t>(-4.615109057004597e-05, 2.9796481139709275e-05)</t>
+          <t>(-2.716419764260716e-05, 1.0809588212270463e-05)</t>
         </is>
       </c>
       <c r="AK3" t="inlineStr">
         <is>
-          <t>(-0.0002481943983235049, 0.0002731338883878143)</t>
+          <t>(-0.00011786232664567507, 0.00014280181670998454)</t>
         </is>
       </c>
     </row>
@@ -9970,112 +9970,112 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>(-3.339372982140261e-05, -1.371593949672967e-05)</t>
+          <t>(-2.847428224023437e-05, -1.8635387077897906e-05)</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>(0.08054503376133818, 0.16721150679418573)</t>
+          <t>(0.10221165201955007, 0.14554488853597383)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>(0.031010833047676975, 0.03934167260600645)</t>
+          <t>(0.03309354293725934, 0.03725896271642408)</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>(0.0015142674255694158, 0.00601026700182042)</t>
+          <t>(0.002638267319632167, 0.00488626710775767)</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>(0.0737660059933779, 0.08419099605774033)</t>
+          <t>(0.07637225350946851, 0.08158474854164972)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>(-0.02138333912762265, -0.01015716472458253)</t>
+          <t>(-0.01857679552686262, -0.01296370832534256)</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>(-0.1334029023178348, -0.08682820724377222)</t>
+          <t>(-0.12175922854931916, -0.09847188101228786)</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(0.005906965510080936, 0.019177260458170253)</t>
+          <t>(0.009224539247103265, 0.015859686721147924)</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>(0.0006646953968776263, 0.002374972874558924)</t>
+          <t>(0.0010922647662979508, 0.0019474035051385992)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>(0.0054655581096564945, 0.007097063277299325)</t>
+          <t>(0.0058734344015672025, 0.006689186985388617)</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>(-0.004644826664127502, -0.002366883538332979)</t>
+          <t>(-0.004075340882678871, -0.00293636931978161)</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>(-0.1595928536970427, 0.0839084058677168)</t>
+          <t>(-0.09871753880585282, 0.023033090976526928)</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>(0.02633981240223259, 0.03602367566665788)</t>
+          <t>(0.028760778218338914, 0.03360270985055156)</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>(-0.0003611542845756043, 0.0007701038360814751)</t>
+          <t>(-7.833975441133445e-05, 0.0004872893059172052)</t>
         </is>
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t>(-0.5437348877240656, -0.060399256174184485)</t>
+          <t>(-0.42290097983659536, -0.1812331640616548)</t>
         </is>
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>(0.007341929559570109, 0.018975328871474552)</t>
+          <t>(0.01025027938754622, 0.016066979043498443)</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>(-0.13304228543546942, -0.08501576576816904)</t>
+          <t>(-0.12103565551864433, -0.09702239568499414)</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>(0.014004884233067356, 0.02165597751771935)</t>
+          <t>(0.015917657554230354, 0.01974320419655635)</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
         <is>
-          <t>(-0.007699928511012091, -0.006085130030522815)</t>
+          <t>(-0.007296228890889772, -0.006488829650645135)</t>
         </is>
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t>(-0.004263223252915094, 0.0005174061691585272)</t>
+          <t>(-0.003068065897396689, -0.0006777511863598781)</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
         <is>
-          <t>(-0.02073333720997006, -0.0069952613192373345)</t>
+          <t>(-0.017298818237286878, -0.010429780291920515)</t>
         </is>
       </c>
       <c r="W4" t="inlineStr">
         <is>
-          <t>(-0.0007113812175936927, 0.0014614290752946548)</t>
+          <t>(-0.00016817864437160577, 0.000918226502072568)</t>
         </is>
       </c>
       <c r="X4" t="inlineStr">
@@ -10085,12 +10085,12 @@
       </c>
       <c r="Y4" t="inlineStr">
         <is>
-          <t>(-0.03146586734447579, -0.012231501985157886)</t>
+          <t>(-0.02665727600464631, -0.017040093324987363)</t>
         </is>
       </c>
       <c r="Z4" t="inlineStr">
         <is>
-          <t>(-0.028389695619724074, -0.019016933303777527)</t>
+          <t>(-0.02604650504073744, -0.021360123882764162)</t>
         </is>
       </c>
       <c r="AA4" t="inlineStr">
@@ -10100,52 +10100,52 @@
       </c>
       <c r="AB4" t="inlineStr">
         <is>
-          <t>(-0.008174350811815934, -0.004665004139649461)</t>
+          <t>(-0.0072970141437743155, -0.00554234080769108)</t>
         </is>
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>(-0.013512354171676393, -0.0056516419133044995)</t>
+          <t>(-0.01154717610708342, -0.0076168199778974734)</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>(-0.053572687944894906, -0.009215748993311804)</t>
+          <t>(-0.04248345320699913, -0.02030498373120758)</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>(0.007648896770734569, 0.02376557109544738)</t>
+          <t>(0.011678065351912771, 0.019736402514269176)</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>(0.03734940046351206, 0.0615398862733011)</t>
+          <t>(0.04339702191595932, 0.055492264820853836)</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>(-0.07873673970553234, -0.054483874227397075)</t>
+          <t>(-0.07267352333599852, -0.06054709059693089)</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>(-0.020954544637308885, -0.01450284996405165)</t>
+          <t>(-0.019341620968994576, -0.016115773632365958)</t>
         </is>
       </c>
       <c r="AI4" t="inlineStr">
         <is>
-          <t>(-0.005028891527772841, -0.0017402086205009744)</t>
+          <t>(-0.004206720800954874, -0.002562379347318941)</t>
         </is>
       </c>
       <c r="AJ4" t="inlineStr">
         <is>
-          <t>(-0.01150315943369994, -0.003283607154444694)</t>
+          <t>(-0.009448271363886127, -0.005338495224258505)</t>
         </is>
       </c>
       <c r="AK4" t="inlineStr">
         <is>
-          <t>(-0.023821282093209134, -0.009931494945523875)</t>
+          <t>(-0.020348835306287817, -0.01340394173244519)</t>
         </is>
       </c>
     </row>
@@ -10157,127 +10157,127 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>(-0.00012956494052639156, 0.0003250269009056304)</t>
+          <t>(-1.5916980168386086e-05, 0.00021137894054762489)</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>(-0.030456294955128436, -0.009652931689841231)</t>
+          <t>(-0.025255454138806633, -0.014853772506163033)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>(0.008789421232688058, 0.02182216233199265)</t>
+          <t>(0.012047606507514207, 0.018563977057166503)</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>(0.0021683508322746944, 0.003731236817294222)</t>
+          <t>(0.0025590723285295763, 0.00334051532103934)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>(-0.020105562426404704, 0.04638426972082826)</t>
+          <t>(-0.0034831043895964635, 0.029761811684020017)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>(-0.005996658278096678, -0.0006442774301652909)</t>
+          <t>(-0.004658563066113831, -0.0019823726421481377)</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>(-0.025948409971890338, 0.00215016879551669)</t>
+          <t>(-0.018923765280038578, -0.004874475896335067)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(-0.0028264530063613963, -0.0011509055789274182)</t>
+          <t>(-0.0024075661495029017, -0.0015697924357859125)</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>(0.00027818593941081413, 0.0018515656833241892)</t>
+          <t>(0.0006715308753891579, 0.0014582207473458455)</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>(0.0010541373571523937, 0.00243975129539833)</t>
+          <t>(0.0014005408417138777, 0.0020933478108368458)</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>(-0.0006011010377767757, 3.633486927036257e-05)</t>
+          <t>(-0.0004417420610149911, -0.000123024107491422)</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>(-0.008737171355962246, 0.009498968234928845)</t>
+          <t>(-0.004178136458239472, 0.0049399333372060735)</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>(0.001985386276846854, 0.011502694133088211)</t>
+          <t>(0.004364713240907194, 0.009123367169027872)</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>(-4.0776085748969764e-05, 0.000152339166508771)</t>
+          <t>(7.502727315465426e-06, 0.00010406035344433581)</t>
         </is>
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t>(-0.15197802937356847, -0.029542212936079906)</t>
+          <t>(-0.12136907526419634, -0.06015116704545205)</t>
         </is>
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>(-1.6017967615051783e-05, 0.0012730119032051102)</t>
+          <t>(0.0003062395000899887, 0.0009507544355000697)</t>
         </is>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>(-0.015796709415538665, 0.004299897992249101)</t>
+          <t>(-0.010772557563591722, -0.00072425385969784)</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>(0.0027242299899624357, 0.00877377507941449)</t>
+          <t>(0.00423661626232545, 0.0072613888070514766)</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>(-0.0022292564084970016, -0.00021896421662403326)</t>
+          <t>(-0.0017266833605287595, -0.0007215372645922753)</t>
         </is>
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t>(-0.0006065761281136662, 0.0004961034869047949)</t>
+          <t>(-0.00033090622435905093, 0.00022043358315017962)</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>(-0.006941835817616565, -0.0017172188852326875)</t>
+          <t>(-0.005635681584520595, -0.003023373118328657)</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
         <is>
-          <t>(0.0009450301616817945, 0.0014719167273984117)</t>
+          <t>(0.0010767518031109488, 0.0013401950859692575)</t>
         </is>
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>(0.0005620252157100061, 0.0038093056934087703)</t>
+          <t>(0.0013738453351346972, 0.0029974855739840793)</t>
         </is>
       </c>
       <c r="Y5" t="inlineStr">
         <is>
-          <t>(-0.010474518888271396, -0.002364050153059942)</t>
+          <t>(-0.008446901704468534, -0.004391667336862805)</t>
         </is>
       </c>
       <c r="Z5" t="inlineStr">
         <is>
-          <t>(-0.007270478083482412, -0.0009747895178779651)</t>
+          <t>(-0.0056965559420813, -0.002548711659279077)</t>
         </is>
       </c>
       <c r="AA5" t="inlineStr">
@@ -10287,52 +10287,52 @@
       </c>
       <c r="AB5" t="inlineStr">
         <is>
-          <t>(-0.0022878305568552987, -0.0004310401304309762)</t>
+          <t>(-0.001823632950249218, -0.0008952377370370567)</t>
         </is>
       </c>
       <c r="AC5" t="inlineStr">
         <is>
-          <t>(-0.003410491782704807, -0.0006664294049153578)</t>
+          <t>(-0.0027244761882574448, -0.0013524449993627201)</t>
         </is>
       </c>
       <c r="AD5" t="inlineStr">
         <is>
-          <t>(-0.006038278413282431, -0.001021041902309912)</t>
+          <t>(-0.004783969285539301, -0.0022753510300530418)</t>
         </is>
       </c>
       <c r="AE5" t="inlineStr">
         <is>
-          <t>(0.0011434295586430236, 0.003729310006231116)</t>
+          <t>(0.0017898996705400468, 0.003082839894334093)</t>
         </is>
       </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>(-0.01580387234916942, -0.010500304974753214)</t>
+          <t>(-0.014477980505565367, -0.011826196818357266)</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>(-0.02220316180766868, -0.001285275451851177)</t>
+          <t>(-0.016973690218714303, -0.006514747040805553)</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>(-0.004276852145340979, -0.001118673517515622)</t>
+          <t>(-0.00348730748838464, -0.0019082181744719613)</t>
         </is>
       </c>
       <c r="AI5" t="inlineStr">
         <is>
-          <t>(-0.0014156139382845911, -0.0004805643052599376)</t>
+          <t>(-0.0011818515300284279, -0.000714326713516101)</t>
         </is>
       </c>
       <c r="AJ5" t="inlineStr">
         <is>
-          <t>(-0.002631437318143762, -0.0004019828608080051)</t>
+          <t>(-0.002074073703809823, -0.0009593464751419444)</t>
         </is>
       </c>
       <c r="AK5" t="inlineStr">
         <is>
-          <t>(-0.007264075666097932, -0.0017304175209537924)</t>
+          <t>(-0.005880661129811897, -0.003113832057239827)</t>
         </is>
       </c>
     </row>
@@ -10344,127 +10344,127 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>(-9.232775559139095e-05, 4.614021268468195e-05)</t>
+          <t>(-5.771076352237273e-05, 1.1523220615663722e-05)</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>(0.0008192795385873032, 0.00504979585929771)</t>
+          <t>(0.001876908618764905, 0.003992166779120109)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>(0.0018994199070588875, 0.009132277761686057)</t>
+          <t>(0.00370763437071568, 0.007324063298029265)</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>(0.0007297152207300425, 0.002969180382138514)</t>
+          <t>(0.0012895815110821602, 0.0024093140917863963)</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>(-0.0117890326438152, 0.00031839774977569183)</t>
+          <t>(-0.008762175045417476, -0.002708459848622031)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>(-0.0008426317520851254, -0.00012113259071368796)</t>
+          <t>(-0.0006622569617422661, -0.00030150738105654733)</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>(-0.0015606392360416773, -0.0004965413537901468)</t>
+          <t>(-0.0012946147654787946, -0.0007625658243530294)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(-0.0012533383476789996, -0.0001894047648756537)</t>
+          <t>(-0.0009873549519781631, -0.0004553881605764902)</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>(6.757758607532323e-05, 0.0003653035079415029)</t>
+          <t>(0.00014200906654186817, 0.000290872027474958)</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>(7.096716541697695e-05, 0.0007646219880246316)</t>
+          <t>(0.0002443808710688906, 0.0005912082823727178)</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>(-5.704074812840437e-05, -1.6870384233212294e-05)</t>
+          <t>(-4.699815715460635e-05, -2.6912975207010315e-05)</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
         <is>
-          <t>(-0.0013639973562469894, 0.0016704780930380434)</t>
+          <t>(-0.0006053784939257312, 0.0009118592307167852)</t>
         </is>
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>(0.00021486049595104638, 0.0021980812325190866)</t>
+          <t>(0.0007106656800930564, 0.0017022760483770764)</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>(-1.3295494785972614e-05, 4.8046240319966124e-05)</t>
+          <t>(2.0399389905120695e-06, 3.271080654348143e-05)</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>(-0.035670797261939245, -0.010904603699409843)</t>
+          <t>(-0.029479248871306894, -0.017096152090042192)</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>(0.0003079162818469312, 0.0009341935076698132)</t>
+          <t>(0.0004644855883026517, 0.0007776242012140927)</t>
         </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
-          <t>(-0.00016289013590111448, 6.955945912391414e-06)</t>
+          <t>(-0.000120428615447738, -3.550557454098506e-05)</t>
         </is>
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>(0.0006023951857923033, 0.002408460427661525)</t>
+          <t>(0.0010539114962596088, 0.0019569441171942196)</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>(-0.0002665751922675826, -3.0060161291398565e-05)</t>
+          <t>(-0.0002074464345235366, -8.918891903544459e-05)</t>
         </is>
       </c>
       <c r="U6" t="inlineStr">
         <is>
-          <t>(-1.6945722011892637e-05, 0.00025405710177132696)</t>
+          <t>(5.080498393391226e-05, 0.00018630639582552206)</t>
         </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
-          <t>(-0.001377567320681401, -0.0003876557849792348)</t>
+          <t>(-0.0011300894367558595, -0.0006351336689047764)</t>
         </is>
       </c>
       <c r="W6" t="inlineStr">
         <is>
-          <t>(0.00046239881683828477, 0.0014066878445351295)</t>
+          <t>(0.000698471073762496, 0.0011706155876109185)</t>
         </is>
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>(-4.420554141625654e-06, 0.00014169279739466176)</t>
+          <t>(3.21077837424462e-05, 0.00010516445951058991)</t>
         </is>
       </c>
       <c r="Y6" t="inlineStr">
         <is>
-          <t>(-0.0023760673976150515, -0.00069131715369625)</t>
+          <t>(-0.0019548798366353514, -0.0011125047146759504)</t>
         </is>
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>(-0.0012534499818150384, -0.00011893251517170833)</t>
+          <t>(-0.0009698206151542057, -0.0004025618818325408)</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
@@ -10474,52 +10474,52 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>(-0.00038986649958619506, -6.26127269921282e-05)</t>
+          <t>(-0.00030805305643767834, -0.00014442617014064492)</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>(-0.0004744748953184163, -0.00011834352684764006)</t>
+          <t>(-0.00038544205320072226, -0.00020737636896533414)</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
         <is>
-          <t>(-0.0011851806750739938, 2.1992580385846346e-05)</t>
+          <t>(-0.0008833873612090337, -0.0002798007334791137)</t>
         </is>
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>(0.00013027083752614895, 0.001423519714717042)</t>
+          <t>(0.00045358305682387224, 0.0011002074954193188)</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>(-0.0008657222478792078, 0.00013351379289073374)</t>
+          <t>(-0.0006159132376867225, -0.00011629521730175166)</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>(-0.0025763975206741416, -0.0005703516650957677)</t>
+          <t>(-0.0020748860567795483, -0.001071863128990361)</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
         <is>
-          <t>(-0.0007652239377534172, -0.00013550340980241317)</t>
+          <t>(-0.0006077938057656662, -0.00029293354179016416)</t>
         </is>
       </c>
       <c r="AI6" t="inlineStr">
         <is>
-          <t>(-0.0004064879559603189, -7.155858724658244e-05)</t>
+          <t>(-0.0003227556137818848, -0.00015529092942501656)</t>
         </is>
       </c>
       <c r="AJ6" t="inlineStr">
         <is>
-          <t>(-0.00044705548568855905, -5.6608653247989025e-05)</t>
+          <t>(-0.00034944377757841654, -0.0001542203613581315)</t>
         </is>
       </c>
       <c r="AK6" t="inlineStr">
         <is>
-          <t>(-0.0013956436996273506, -0.0003620016083334066)</t>
+          <t>(-0.0011372331768038646, -0.0006204121311568926)</t>
         </is>
       </c>
     </row>
@@ -10531,52 +10531,52 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>(-0.0001334065405453808, 2.9474198727212884e-05)</t>
+          <t>(-9.268635572723239e-05, -1.1245986090935542e-05)</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>(-0.003058810691542754, -0.00015349447024909303)</t>
+          <t>(-0.0023324816362193385, -0.0008798235255725082)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>(-0.011592293801563094, -5.294372962835834e-05)</t>
+          <t>(-0.008707456283579409, -0.002937781247612042)</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>(-0.01700029852319422, 0.0007246131081677949)</t>
+          <t>(-0.012569070615353716, -0.0037066147996727087)</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>(-0.0006578410216790477, 0.0002115871255775968)</t>
+          <t>(-0.00044048398486488656, -5.769911236564319e-06)</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>(-0.00033697308163710567, 0.00016730203308478324)</t>
+          <t>(-0.00021090430295663343, 4.1233254404311016e-05)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>(-2.6134389303984334e-05, 4.585175148141208e-05)</t>
+          <t>(-8.13785410763523e-06, 2.7855216285062976e-05)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(-5.727012490703643e-05, 0.0026416467072636115)</t>
+          <t>(0.0006174590831356256, 0.0019669174992209496)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>(-0.0008185781148167353, 4.373685164272038e-05)</t>
+          <t>(-0.0006029993732018713, -0.00017184188997214353)</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>(-0.00016673058440547228, 0.0001683308695406553)</t>
+          <t>(-8.296522091894037e-05, 8.456550605412343e-05)</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -10586,127 +10586,127 @@
       </c>
       <c r="M7" t="inlineStr">
         <is>
-          <t>(-0.0006892700885912238, 0.0032895105256935393)</t>
+          <t>(0.00030542506497996695, 0.0022948153721223485)</t>
         </is>
       </c>
       <c r="N7" t="inlineStr">
         <is>
-          <t>(-0.00011942937958637047, 0.001008603026745923)</t>
+          <t>(0.0001625787219967029, 0.0007265949251628497)</t>
         </is>
       </c>
       <c r="O7" t="inlineStr">
         <is>
-          <t>(-0.0002770134942352724, 4.9587136675541434e-05)</t>
+          <t>(-0.00019536333650756893, -3.2063021052162015e-05)</t>
         </is>
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t>(-0.003531921674140473, 0.09567554161668866)</t>
+          <t>(0.02126994414856681, 0.07087367579398138)</t>
         </is>
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>(-0.00243700929345723, 0.0007138189121890323)</t>
+          <t>(-0.0016493022420456644, -7.388813922253328e-05)</t>
         </is>
       </c>
       <c r="R7" t="inlineStr">
         <is>
-          <t>(-0.00010901111631715238, 3.209319141318506e-05)</t>
+          <t>(-7.373503938456802e-05, -3.182885519399301e-06)</t>
         </is>
       </c>
       <c r="S7" t="inlineStr">
         <is>
-          <t>(-0.004117712193294904, 0.00039364181421493714)</t>
+          <t>(-0.002989873691417444, -0.0007341966876625232)</t>
         </is>
       </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>(-0.00014061550078106207, 8.697627803039802e-05)</t>
+          <t>(-8.371755607819705e-05, 3.0078333327532997e-05)</t>
         </is>
       </c>
       <c r="U7" t="inlineStr">
         <is>
-          <t>(-0.0002927335123836016, 0.0001820485945370162)</t>
+          <t>(-0.00017403798565344714, 6.335306780686174e-05)</t>
         </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
-          <t>(-1.589634323771597e-05, 0.0018135317986396325)</t>
+          <t>(0.0004414606922316211, 0.0013561747631702953)</t>
         </is>
       </c>
       <c r="W7" t="inlineStr">
         <is>
-          <t>(-0.0025727031847126254, 6.761716316965038e-07)</t>
+          <t>(-0.001929358345626545, -0.000642668667454384)</t>
         </is>
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>(-0.0020435335526046384, 0.0002487442465430288)</t>
+          <t>(-0.0014704641028177217, -0.00032432520324388806)</t>
         </is>
       </c>
       <c r="Y7" t="inlineStr">
         <is>
-          <t>(3.3020484702835085e-06, 0.002607848033311112)</t>
+          <t>(0.0006544385446804906, 0.001956711537100905)</t>
         </is>
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>(-0.0003591089394221371, 0.00011583845836968202)</t>
+          <t>(-0.00024037208997418233, -2.898391078272764e-06)</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
-          <t>(-0.0008960095917417315, 0.0002498989867401548)</t>
+          <t>(-0.0006095324471212599, -3.6578157880316786e-05)</t>
         </is>
       </c>
       <c r="AB7" t="inlineStr">
         <is>
-          <t>(-2.042885365335352e-05, 0.0002003506845085465)</t>
+          <t>(3.476603088712148e-05, 0.00014515579996807147)</t>
         </is>
       </c>
       <c r="AC7" t="inlineStr">
         <is>
-          <t>(-1.982183154377813e-05, 0.00023201028112322756)</t>
+          <t>(4.313619662297329e-05, 0.00016905225295647613)</t>
         </is>
       </c>
       <c r="AD7" t="inlineStr">
         <is>
-          <t>(-0.0007154340322072814, 0.00030342626848506776)</t>
+          <t>(-0.0004607189570341941, 4.8711193311980466e-05)</t>
         </is>
       </c>
       <c r="AE7" t="inlineStr">
         <is>
-          <t>(-0.004551830702258797, 0.00015196491466086277)</t>
+          <t>(-0.003375881798028882, -0.0010239839895690521)</t>
         </is>
       </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>(-0.00034779976008027973, 2.61929697618413e-05)</t>
+          <t>(-0.0002543015776197495, -6.730521269868896e-05)</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>(-0.0005836107932710691, 0.000271380518093023)</t>
+          <t>(-0.000369862965430046, 5.7632690252000014e-05)</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
         <is>
-          <t>(-0.0001437827835618802, 0.0006159309591818346)</t>
+          <t>(4.6145652124048514e-05, 0.0004260025234959059)</t>
         </is>
       </c>
       <c r="AI7" t="inlineStr">
         <is>
-          <t>(2.7775601812115506e-05, 0.0007943324627030051)</t>
+          <t>(0.0002194148170348379, 0.0006026932474802826)</t>
         </is>
       </c>
       <c r="AJ7" t="inlineStr">
         <is>
-          <t>(-5.80383608406929e-05, 0.0001369618868425639)</t>
+          <t>(-9.2882989198787e-06, 8.82118249217497e-05)</t>
         </is>
       </c>
       <c r="AK7" t="inlineStr">
         <is>
-          <t>(1.1965464626772344e-05, 0.001299996628530628)</t>
+          <t>(0.0003339732556027363, 0.0009779888375546642)</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates on specific rates calculation with the values from metabolite analyzer
</commit_message>
<xml_diff>
--- a/Data/ZeLa Data/specific_rates_R.xlsx
+++ b/Data/ZeLa Data/specific_rates_R.xlsx
@@ -6310,7 +6310,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6331,175 +6331,195 @@
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>NH4</t>
+          <t>Glucose (Met)</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
+          <t>Glutamate (Met)</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Glutamine (Met)</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Lactate (Met)</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>NH4 (Met)</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
           <t>SGR</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>acetic acid</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>alanine</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>arginine</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>asparagine</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>aspartic acid</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>butyric &amp; 2-hydroxy- butyric acids</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>citric acid</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>cystine</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>ethanol</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>formic acid</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>fumaric acid</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>glutamic acid</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>glutamine</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>glycine</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>histidine</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>hydroxyproline</t>
         </is>
       </c>
-      <c r="V1" s="4" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>isoleucine</t>
         </is>
       </c>
-      <c r="W1" s="4" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>isovaleric acid</t>
         </is>
       </c>
-      <c r="X1" s="4" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>lactic acid</t>
         </is>
       </c>
-      <c r="Y1" s="4" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>leucine</t>
         </is>
       </c>
-      <c r="Z1" s="4" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>lysine</t>
         </is>
       </c>
-      <c r="AA1" s="4" t="inlineStr">
+      <c r="AE1" s="4" t="inlineStr">
         <is>
           <t>malic acid</t>
         </is>
       </c>
-      <c r="AB1" s="4" t="inlineStr">
+      <c r="AF1" s="4" t="inlineStr">
         <is>
           <t>methionine</t>
         </is>
       </c>
-      <c r="AC1" s="4" t="inlineStr">
+      <c r="AG1" s="4" t="inlineStr">
         <is>
           <t>phenylalanine</t>
         </is>
       </c>
-      <c r="AD1" s="4" t="inlineStr">
+      <c r="AH1" s="4" t="inlineStr">
         <is>
           <t>proline</t>
         </is>
       </c>
-      <c r="AE1" s="4" t="inlineStr">
+      <c r="AI1" s="4" t="inlineStr">
         <is>
           <t>pyroglutamic acid</t>
         </is>
       </c>
-      <c r="AF1" s="4" t="inlineStr">
+      <c r="AJ1" s="4" t="inlineStr">
         <is>
           <t>pyruvic acid</t>
         </is>
       </c>
-      <c r="AG1" s="4" t="inlineStr">
+      <c r="AK1" s="4" t="inlineStr">
         <is>
           <t>serine</t>
         </is>
       </c>
-      <c r="AH1" s="4" t="inlineStr">
+      <c r="AL1" s="4" t="inlineStr">
         <is>
           <t>threonine</t>
         </is>
       </c>
-      <c r="AI1" s="4" t="inlineStr">
+      <c r="AM1" s="4" t="inlineStr">
         <is>
           <t>tryptophan</t>
         </is>
       </c>
-      <c r="AJ1" s="4" t="inlineStr">
+      <c r="AN1" s="4" t="inlineStr">
         <is>
           <t>tyrosine</t>
         </is>
       </c>
-      <c r="AK1" s="4" t="inlineStr">
+      <c r="AO1" s="4" t="inlineStr">
         <is>
           <t>valine</t>
         </is>
@@ -6515,108 +6535,120 @@
         <v>0.01088765852742637</v>
       </c>
       <c r="C2" t="n">
+        <v>-1.076030475392915</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.02814899053539199</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.3721631139368082</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2.070590951829618</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.3923591174822987</v>
       </c>
-      <c r="D2" t="n">
+      <c r="H2" t="n">
         <v>0.03573083637649191</v>
       </c>
-      <c r="E2" t="n">
+      <c r="I2" t="n">
         <v>0.019311899556554</v>
       </c>
-      <c r="F2" t="n">
+      <c r="J2" t="n">
         <v>0.1698026792391464</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
         <v>-0.02318991507420184</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L2" t="n">
         <v>-0.2285830065069847</v>
       </c>
-      <c r="I2" t="n">
+      <c r="M2" t="n">
         <v>0.03866677824486502</v>
       </c>
-      <c r="J2" t="n">
+      <c r="N2" t="n">
         <v>0.01307581470561753</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
         <v>-0.01256598310835759</v>
       </c>
-      <c r="M2" t="n">
+      <c r="Q2" t="n">
         <v>0.06481372932408556</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>0.1010220759976825</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>-0.4551226630824849</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="U2" t="n">
         <v>0.02891453777180399</v>
       </c>
-      <c r="R2" t="n">
+      <c r="V2" t="n">
         <v>-0.6368315178380607</v>
       </c>
-      <c r="S2" t="n">
+      <c r="W2" t="n">
         <v>0.03230113784599355</v>
       </c>
-      <c r="T2" t="n">
+      <c r="X2" t="n">
         <v>-0.007023181939971931</v>
       </c>
-      <c r="U2" t="n">
+      <c r="Y2" t="n">
         <v>-0.007891885561453486</v>
       </c>
-      <c r="V2" t="n">
+      <c r="Z2" t="n">
         <v>-0.01952969598606246</v>
       </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
         <v>1.876989705779608</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AC2" t="n">
         <v>-0.03352629271010098</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AD2" t="n">
         <v>-0.03217272821885322</v>
       </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="n">
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
         <v>-0.01345518108242</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AG2" t="n">
         <v>0.001158757564478861</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AH2" t="n">
         <v>0.1073580146241148</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AI2" t="n">
         <v>0.3033395275567397</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AJ2" t="n">
         <v>-0.0816552306269423</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AK2" t="n">
         <v>-0.1565675442136588</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AL2" t="n">
         <v>-0.0194159325524488</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AM2" t="n">
         <v>-0.008874213841584395</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AN2" t="n">
         <v>0.01205655345941475</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AO2" t="n">
         <v>-0.02812847883935459</v>
       </c>
     </row>
@@ -6630,108 +6662,120 @@
         <v>0.0006652198784696813</v>
       </c>
       <c r="C3" t="n">
+        <v>-0.2691266020995701</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.005055772999066666</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.1985270286203769</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.01325663938728722</v>
       </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
         <v>-0.001979179918725814</v>
       </c>
-      <c r="E3" t="n">
+      <c r="I3" t="n">
         <v>0.08444569887822695</v>
       </c>
-      <c r="F3" t="n">
+      <c r="J3" t="n">
         <v>-0.001256910479518427</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
         <v>0.00133883123250859</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
         <v>-0.001773847067767791</v>
       </c>
-      <c r="J3" t="n">
+      <c r="N3" t="n">
         <v>0.0001112226046883693</v>
       </c>
-      <c r="K3" t="n">
+      <c r="O3" t="n">
         <v>-0.0006435715275151789</v>
       </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>-0.006803449710629825</v>
       </c>
-      <c r="N3" t="n">
+      <c r="R3" t="n">
         <v>-0.002160919964997687</v>
       </c>
-      <c r="O3" t="n">
+      <c r="S3" t="n">
         <v>0.0003962333941035079</v>
       </c>
-      <c r="P3" t="n">
+      <c r="T3" t="n">
         <v>-0.1602118984244247</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="U3" t="n">
         <v>-0.0005652650020581809</v>
       </c>
-      <c r="R3" t="n">
+      <c r="V3" t="n">
         <v>-3.267502776793677e-05</v>
       </c>
-      <c r="S3" t="n">
+      <c r="W3" t="n">
         <v>0.009121342020974938</v>
       </c>
-      <c r="T3" t="n">
+      <c r="X3" t="n">
         <v>0.0003224321441093135</v>
       </c>
-      <c r="U3" t="n">
+      <c r="Y3" t="n">
         <v>0.004150268519991077</v>
       </c>
-      <c r="V3" t="n">
+      <c r="Z3" t="n">
         <v>0.0005158491746149783</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AA3" t="n">
         <v>0.0007646785373984512</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AB3" t="n">
         <v>0.1264094846766559</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="AC3" t="n">
         <v>0.000867597677468091</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AD3" t="n">
         <v>0.002001341888853073</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AE3" t="n">
         <v>0.0008983227332730655</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AF3" t="n">
         <v>0.0005735838906816244</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AG3" t="n">
         <v>0.0002816938669566906</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AH3" t="n">
         <v>0.004434887437408095</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AI3" t="n">
         <v>0.003189256673861871</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AJ3" t="n">
         <v>0.000149362184165549</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AK3" t="n">
         <v>0.0002916899520229034</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AL3" t="n">
         <v>0.001733356906510207</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AM3" t="n">
         <v>0.0001275819234946795</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AN3" t="n">
         <v>1.731521672040575e-05</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="AO3" t="n">
         <v>0.0006885766796165116</v>
       </c>
     </row>
@@ -6745,108 +6789,120 @@
         <v>0.004250930319835426</v>
       </c>
       <c r="C4" t="n">
+        <v>-0.5568743780993389</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01607931349766054</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.09455813630085891</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.7089885652960982</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.1183501638854216</v>
       </c>
-      <c r="D4" t="n">
+      <c r="H4" t="n">
         <v>0.03424980254030179</v>
       </c>
-      <c r="E4" t="n">
+      <c r="I4" t="n">
         <v>0.001473421673937969</v>
       </c>
-      <c r="F4" t="n">
+      <c r="J4" t="n">
         <v>0.05895667873313951</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
         <v>-0.0192351172892534</v>
       </c>
-      <c r="H4" t="n">
+      <c r="L4" t="n">
         <v>-0.1149674855122498</v>
       </c>
-      <c r="I4" t="n">
+      <c r="M4" t="n">
         <v>0.01998852975044968</v>
       </c>
-      <c r="J4" t="n">
+      <c r="N4" t="n">
         <v>0.001571949836822859</v>
       </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
         <v>0.007626706485194226</v>
       </c>
-      <c r="L4" t="n">
+      <c r="P4" t="n">
         <v>-0.003963709998101374</v>
       </c>
-      <c r="M4" t="n">
+      <c r="Q4" t="n">
         <v>0.05157902268896466</v>
       </c>
-      <c r="N4" t="n">
+      <c r="R4" t="n">
         <v>0.03304772144004316</v>
       </c>
-      <c r="O4" t="n">
+      <c r="S4" t="n">
         <v>0.0002418629456945973</v>
       </c>
-      <c r="P4" t="n">
+      <c r="T4" t="n">
         <v>-0.6091132688163742</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="U4" t="n">
         <v>0.01455829738150945</v>
       </c>
-      <c r="R4" t="n">
+      <c r="V4" t="n">
         <v>-0.1224288471039342</v>
       </c>
-      <c r="S4" t="n">
+      <c r="W4" t="n">
         <v>0.01522999196671617</v>
       </c>
-      <c r="T4" t="n">
+      <c r="X4" t="n">
         <v>-0.007197445809596336</v>
       </c>
-      <c r="U4" t="n">
+      <c r="Y4" t="n">
         <v>-0.002767468016015338</v>
       </c>
-      <c r="V4" t="n">
+      <c r="Z4" t="n">
         <v>-0.01659101614595327</v>
       </c>
-      <c r="W4" t="n">
+      <c r="AA4" t="n">
         <v>0.000647373385167743</v>
       </c>
-      <c r="X4" t="n">
+      <c r="AB4" t="n">
         <v>0.8628761344641598</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="AC4" t="n">
         <v>-0.0274771620768797</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AD4" t="n">
         <v>-0.02742356159950963</v>
       </c>
-      <c r="AA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="n">
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
         <v>-0.008881435308065509</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AG4" t="n">
         <v>-0.01076419564886847</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AH4" t="n">
         <v>-0.04184659116281986</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AI4" t="n">
         <v>0.01179620667953501</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AJ4" t="n">
         <v>0.004269695769462214</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AK4" t="n">
         <v>-0.06849475908508246</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AL4" t="n">
         <v>-0.02122144728417101</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AM4" t="n">
         <v>-0.003982321267988898</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AN4" t="n">
         <v>-0.01251424269696163</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AO4" t="n">
         <v>-0.02274972240105925</v>
       </c>
     </row>
@@ -6860,108 +6916,120 @@
         <v>0.0009789568708174817</v>
       </c>
       <c r="C5" t="n">
+        <v>-0.3112096859122847</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.002687723818444813</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.01426653739615039</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1170111569730567</v>
+      </c>
+      <c r="G5" t="n">
         <v>-0.005429718853254245</v>
       </c>
-      <c r="D5" t="n">
+      <c r="H5" t="n">
         <v>0.0168847193685378</v>
       </c>
-      <c r="E5" t="n">
+      <c r="I5" t="n">
         <v>0.01526503544407851</v>
       </c>
-      <c r="F5" t="n">
+      <c r="J5" t="n">
         <v>0.008877005943595168</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
         <v>-0.008799821364029148</v>
       </c>
-      <c r="H5" t="n">
+      <c r="L5" t="n">
         <v>-0.03653673154794896</v>
       </c>
-      <c r="I5" t="n">
+      <c r="M5" t="n">
         <v>-0.003456882176772502</v>
       </c>
-      <c r="J5" t="n">
+      <c r="N5" t="n">
         <v>0.002604987862500291</v>
       </c>
-      <c r="K5" t="n">
+      <c r="O5" t="n">
         <v>0.005716021725071845</v>
       </c>
-      <c r="L5" t="n">
+      <c r="P5" t="n">
         <v>-0.0008156131670001286</v>
       </c>
-      <c r="M5" t="n">
+      <c r="Q5" t="n">
         <v>0.006708160786873816</v>
       </c>
-      <c r="N5" t="n">
+      <c r="R5" t="n">
         <v>0.02043215949099502</v>
       </c>
-      <c r="O5" t="n">
+      <c r="S5" t="n">
         <v>-3.792640395335315e-06</v>
       </c>
-      <c r="P5" t="n">
+      <c r="T5" t="n">
         <v>-0.3085343933127628</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="U5" t="n">
         <v>0.002830702685972168</v>
       </c>
-      <c r="R5" t="n">
+      <c r="V5" t="n">
         <v>-0.01135686479994072</v>
       </c>
-      <c r="S5" t="n">
+      <c r="W5" t="n">
         <v>0.01247633656607483</v>
       </c>
-      <c r="T5" t="n">
+      <c r="X5" t="n">
         <v>-0.003760693065431248</v>
       </c>
-      <c r="U5" t="n">
+      <c r="Y5" t="n">
         <v>-0.001236831631849316</v>
       </c>
-      <c r="V5" t="n">
+      <c r="Z5" t="n">
         <v>-0.01019685189149555</v>
       </c>
-      <c r="W5" t="n">
+      <c r="AA5" t="n">
         <v>0.002156343493245803</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AB5" t="n">
         <v>0.182326577922321</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AC5" t="n">
         <v>-0.01598092646485115</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AD5" t="n">
         <v>-0.01168624359919693</v>
       </c>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="n">
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
         <v>-0.004017726871808334</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AG5" t="n">
         <v>-0.006108166194626238</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AH5" t="n">
         <v>-0.01192674550518479</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AI5" t="n">
         <v>0.002775377055129672</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AJ5" t="n">
         <v>-0.01119020611857758</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AK5" t="n">
         <v>-0.03879790584041778</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AL5" t="n">
         <v>-0.009415633075277881</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AM5" t="n">
         <v>-0.003131909921035302</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AN5" t="n">
         <v>-0.003622879388540588</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AO5" t="n">
         <v>-0.01176260544477364</v>
       </c>
     </row>
@@ -6975,108 +7043,120 @@
         <v>0.0005674184224825113</v>
       </c>
       <c r="C6" t="n">
+        <v>-0.2552810321423932</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.001958795284982216</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.112366412596784</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.01836375734366704</v>
       </c>
-      <c r="D6" t="n">
+      <c r="H6" t="n">
         <v>-0.00182581693798973</v>
       </c>
-      <c r="E6" t="n">
+      <c r="I6" t="n">
         <v>0.05644081634701429</v>
       </c>
-      <c r="F6" t="n">
+      <c r="J6" t="n">
         <v>-0.0182298543824564</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
         <v>-0.002498817045224501</v>
       </c>
-      <c r="H6" t="n">
+      <c r="L6" t="n">
         <v>-0.009719418538976801</v>
       </c>
-      <c r="I6" t="n">
+      <c r="M6" t="n">
         <v>-0.005337054651967852</v>
       </c>
-      <c r="J6" t="n">
+      <c r="N6" t="n">
         <v>0.002605588873126109</v>
       </c>
-      <c r="K6" t="n">
+      <c r="O6" t="n">
         <v>0.003320547033330585</v>
       </c>
-      <c r="L6" t="n">
+      <c r="P6" t="n">
         <v>-0.0003510633000670026</v>
       </c>
-      <c r="M6" t="n">
+      <c r="Q6" t="n">
         <v>-0.01078906706609873</v>
       </c>
-      <c r="N6" t="n">
+      <c r="R6" t="n">
         <v>0.002519880757282052</v>
       </c>
-      <c r="O6" t="n">
+      <c r="S6" t="n">
         <v>0.000300833039591593</v>
       </c>
-      <c r="P6" t="n">
+      <c r="T6" t="n">
         <v>-0.2867143646478332</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="U6" t="n">
         <v>-1.085248298740911e-05</v>
       </c>
-      <c r="R6" t="n">
+      <c r="V6" t="n">
         <v>9.600406626751124e-05</v>
       </c>
-      <c r="S6" t="n">
+      <c r="W6" t="n">
         <v>0.002824922713548552</v>
       </c>
-      <c r="T6" t="n">
+      <c r="X6" t="n">
         <v>-0.00107602849533963</v>
       </c>
-      <c r="U6" t="n">
+      <c r="Y6" t="n">
         <v>0.0004032158649179266</v>
       </c>
-      <c r="V6" t="n">
+      <c r="Z6" t="n">
         <v>-0.004258265569135606</v>
       </c>
-      <c r="W6" t="n">
+      <c r="AA6" t="n">
         <v>0.004015784722959884</v>
       </c>
-      <c r="X6" t="n">
+      <c r="AB6" t="n">
         <v>0.1236290457945105</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AC6" t="n">
         <v>-0.007405634059720177</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AD6" t="n">
         <v>-0.00361596512623994</v>
       </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
         <v>-0.001537532239980623</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AG6" t="n">
         <v>-0.002091842255627324</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AH6" t="n">
         <v>-0.003193677368793035</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AI6" t="n">
         <v>0.002596317689704709</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AJ6" t="n">
         <v>-0.001516796859213573</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AK6" t="n">
         <v>-0.0104377088855785</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AL6" t="n">
         <v>-0.001552199807210814</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AM6" t="n">
         <v>-0.002015083179034671</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AN6" t="n">
         <v>-0.00186563298114887</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="AO6" t="n">
         <v>-0.004444101078136479</v>
       </c>
     </row>
@@ -7090,108 +7170,120 @@
         <v>0.002811072533928706</v>
       </c>
       <c r="C7" t="n">
+        <v>-0.6593168666857534</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.006892731005801132</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.199177560244001</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.002446319874092407</v>
       </c>
-      <c r="D7" t="n">
+      <c r="H7" t="n">
         <v>-0.008494826177384058</v>
       </c>
-      <c r="E7" t="n">
+      <c r="I7" t="n">
         <v>0.1795902332332139</v>
       </c>
-      <c r="F7" t="n">
+      <c r="J7" t="n">
         <v>0.01320067568421442</v>
       </c>
-      <c r="G7" t="n">
+      <c r="K7" t="n">
         <v>-0.0008697749030163637</v>
       </c>
-      <c r="H7" t="n">
+      <c r="L7" t="n">
         <v>-0.0002692114725096392</v>
       </c>
-      <c r="I7" t="n">
+      <c r="M7" t="n">
         <v>-0.0137773434257676</v>
       </c>
-      <c r="J7" t="n">
+      <c r="N7" t="n">
         <v>0.002468717871617818</v>
       </c>
-      <c r="K7" t="n">
+      <c r="O7" t="n">
         <v>-0.00323642724914663</v>
       </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
         <v>-0.00840496736433618</v>
       </c>
-      <c r="N7" t="n">
+      <c r="R7" t="n">
         <v>-0.009619338902268069</v>
       </c>
-      <c r="O7" t="n">
+      <c r="S7" t="n">
         <v>0.002495147528299949</v>
       </c>
-      <c r="P7" t="n">
+      <c r="T7" t="n">
         <v>-0.6186567172853822</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="U7" t="n">
         <v>0.004898968652874892</v>
       </c>
-      <c r="R7" t="n">
+      <c r="V7" t="n">
         <v>0.0005100889313639252</v>
       </c>
-      <c r="S7" t="n">
+      <c r="W7" t="n">
         <v>0.006982841267503481</v>
       </c>
-      <c r="T7" t="n">
+      <c r="X7" t="n">
         <v>-4.521570121389787e-05</v>
       </c>
-      <c r="U7" t="n">
+      <c r="Y7" t="n">
         <v>-0.0006717349335813278</v>
       </c>
-      <c r="V7" t="n">
+      <c r="Z7" t="n">
         <v>-0.003343531374282764</v>
       </c>
-      <c r="W7" t="n">
+      <c r="AA7" t="n">
         <v>0.003217961233706107</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AB7" t="n">
         <v>0.5468270527143478</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AC7" t="n">
         <v>-0.003958336621522749</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AD7" t="n">
         <v>-0.001152508671931391</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AE7" t="n">
         <v>0.007576887405810373</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AF7" t="n">
         <v>-0.0009315617474331215</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AG7" t="n">
         <v>-0.001505909695203661</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AH7" t="n">
         <v>-0.002735113963852672</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AI7" t="n">
         <v>0.007165829601349097</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AJ7" t="n">
         <v>0.002812453930190892</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AK7" t="n">
         <v>0.000666851951122664</v>
       </c>
-      <c r="AH7" t="n">
+      <c r="AL7" t="n">
         <v>-0.0008901187394992922</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AM7" t="n">
         <v>-0.002609912161354972</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AN7" t="n">
         <v>0.0002122601008998239</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="AO7" t="n">
         <v>-0.002481125166637557</v>
       </c>
     </row>
@@ -7206,7 +7298,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK7"/>
+  <dimension ref="A1:AO7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7227,175 +7319,195 @@
       </c>
       <c r="C1" s="4" t="inlineStr">
         <is>
-          <t>NH4</t>
+          <t>Glucose (Met)</t>
         </is>
       </c>
       <c r="D1" s="4" t="inlineStr">
         <is>
+          <t>Glutamate (Met)</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>Glutamine (Met)</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>Lactate (Met)</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>NH4 (Met)</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
           <t>SGR</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>acetic acid</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>alanine</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>arginine</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>asparagine</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>aspartic acid</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>butyric &amp; 2-hydroxy- butyric acids</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>citric acid</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>cystine</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>ethanol</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>formic acid</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>fumaric acid</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>glucose</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>glutamic acid</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="V1" s="4" t="inlineStr">
         <is>
           <t>glutamine</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="W1" s="4" t="inlineStr">
         <is>
           <t>glycine</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="X1" s="4" t="inlineStr">
         <is>
           <t>histidine</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="Y1" s="4" t="inlineStr">
         <is>
           <t>hydroxyproline</t>
         </is>
       </c>
-      <c r="V1" s="4" t="inlineStr">
+      <c r="Z1" s="4" t="inlineStr">
         <is>
           <t>isoleucine</t>
         </is>
       </c>
-      <c r="W1" s="4" t="inlineStr">
+      <c r="AA1" s="4" t="inlineStr">
         <is>
           <t>isovaleric acid</t>
         </is>
       </c>
-      <c r="X1" s="4" t="inlineStr">
+      <c r="AB1" s="4" t="inlineStr">
         <is>
           <t>lactic acid</t>
         </is>
       </c>
-      <c r="Y1" s="4" t="inlineStr">
+      <c r="AC1" s="4" t="inlineStr">
         <is>
           <t>leucine</t>
         </is>
       </c>
-      <c r="Z1" s="4" t="inlineStr">
+      <c r="AD1" s="4" t="inlineStr">
         <is>
           <t>lysine</t>
         </is>
       </c>
-      <c r="AA1" s="4" t="inlineStr">
+      <c r="AE1" s="4" t="inlineStr">
         <is>
           <t>malic acid</t>
         </is>
       </c>
-      <c r="AB1" s="4" t="inlineStr">
+      <c r="AF1" s="4" t="inlineStr">
         <is>
           <t>methionine</t>
         </is>
       </c>
-      <c r="AC1" s="4" t="inlineStr">
+      <c r="AG1" s="4" t="inlineStr">
         <is>
           <t>phenylalanine</t>
         </is>
       </c>
-      <c r="AD1" s="4" t="inlineStr">
+      <c r="AH1" s="4" t="inlineStr">
         <is>
           <t>proline</t>
         </is>
       </c>
-      <c r="AE1" s="4" t="inlineStr">
+      <c r="AI1" s="4" t="inlineStr">
         <is>
           <t>pyroglutamic acid</t>
         </is>
       </c>
-      <c r="AF1" s="4" t="inlineStr">
+      <c r="AJ1" s="4" t="inlineStr">
         <is>
           <t>pyruvic acid</t>
         </is>
       </c>
-      <c r="AG1" s="4" t="inlineStr">
+      <c r="AK1" s="4" t="inlineStr">
         <is>
           <t>serine</t>
         </is>
       </c>
-      <c r="AH1" s="4" t="inlineStr">
+      <c r="AL1" s="4" t="inlineStr">
         <is>
           <t>threonine</t>
         </is>
       </c>
-      <c r="AI1" s="4" t="inlineStr">
+      <c r="AM1" s="4" t="inlineStr">
         <is>
           <t>tryptophan</t>
         </is>
       </c>
-      <c r="AJ1" s="4" t="inlineStr">
+      <c r="AN1" s="4" t="inlineStr">
         <is>
           <t>tyrosine</t>
         </is>
       </c>
-      <c r="AK1" s="4" t="inlineStr">
+      <c r="AO1" s="4" t="inlineStr">
         <is>
           <t>valine</t>
         </is>
@@ -7411,108 +7523,120 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
+        <v>-0.5082603650054142</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.04289242023381354</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-0.3462310745509806</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.4225880695025642</v>
       </c>
-      <c r="D2" t="n">
+      <c r="H2" t="n">
         <v>0.03532498586833046</v>
       </c>
-      <c r="E2" t="n">
+      <c r="I2" t="n">
         <v>0.03192061838042508</v>
       </c>
-      <c r="F2" t="n">
+      <c r="J2" t="n">
         <v>0.1989943085560181</v>
       </c>
-      <c r="G2" t="n">
+      <c r="K2" t="n">
         <v>-0.02726425134387966</v>
       </c>
-      <c r="H2" t="n">
+      <c r="L2" t="n">
         <v>-0.3455188173485218</v>
       </c>
-      <c r="I2" t="n">
+      <c r="M2" t="n">
         <v>0.03378802224424754</v>
       </c>
-      <c r="J2" t="n">
+      <c r="N2" t="n">
         <v>0.01124831111159965</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
+      <c r="O2" t="n">
+        <v>0</v>
+      </c>
+      <c r="P2" t="n">
         <v>-0.01598672855357584</v>
       </c>
-      <c r="M2" t="n">
+      <c r="Q2" t="n">
         <v>0.5296385777864093</v>
       </c>
-      <c r="N2" t="n">
+      <c r="R2" t="n">
         <v>0.126202291945032</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
+      <c r="S2" t="n">
+        <v>0</v>
+      </c>
+      <c r="T2" t="n">
         <v>-0.08651655065657284</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="U2" t="n">
         <v>0.02309288815098045</v>
       </c>
-      <c r="R2" t="n">
+      <c r="V2" t="n">
         <v>-0.6119057666529618</v>
       </c>
-      <c r="S2" t="n">
+      <c r="W2" t="n">
         <v>0.04555401580184291</v>
       </c>
-      <c r="T2" t="n">
+      <c r="X2" t="n">
         <v>-0.01330461417902425</v>
       </c>
-      <c r="U2" t="n">
+      <c r="Y2" t="n">
         <v>-0.01067550416256867</v>
       </c>
-      <c r="V2" t="n">
+      <c r="Z2" t="n">
         <v>-0.02731276223685298</v>
       </c>
-      <c r="W2" t="n">
-        <v>0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y2" t="n">
+      <c r="AA2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC2" t="n">
         <v>-0.04459989709106457</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AD2" t="n">
         <v>-0.03545993203420453</v>
       </c>
-      <c r="AA2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB2" t="n">
+      <c r="AE2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF2" t="n">
         <v>-0.01938751038245504</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AG2" t="n">
         <v>-0.002373111837007641</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AH2" t="n">
         <v>0.08645749393693172</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AI2" t="n">
         <v>0.3333575278669769</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AJ2" t="n">
         <v>0.08762432681695433</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AK2" t="n">
         <v>-0.2048577726538152</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="AL2" t="n">
         <v>-0.04074806357658683</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="AM2" t="n">
         <v>-0.006889002234633032</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="AN2" t="n">
         <v>-0.009529399896206157</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="AO2" t="n">
         <v>-0.03408377546675641</v>
       </c>
     </row>
@@ -7526,108 +7650,120 @@
         <v>0.0001005850785090534</v>
       </c>
       <c r="C3" t="n">
+        <v>-0.1360752038108523</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00574595555923754</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.003045736316922005</v>
       </c>
-      <c r="D3" t="n">
+      <c r="H3" t="n">
         <v>-0.001881359872232759</v>
       </c>
-      <c r="E3" t="n">
+      <c r="I3" t="n">
         <v>0.03318596960919169</v>
       </c>
-      <c r="F3" t="n">
+      <c r="J3" t="n">
         <v>0.0002455443913354273</v>
       </c>
-      <c r="G3" t="n">
+      <c r="K3" t="n">
         <v>0.0008456418160241351</v>
       </c>
-      <c r="H3" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" t="n">
+      <c r="L3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" t="n">
         <v>0.000886528078840664</v>
       </c>
-      <c r="J3" t="n">
+      <c r="N3" t="n">
         <v>0.0005646256912209101</v>
       </c>
-      <c r="K3" t="n">
+      <c r="O3" t="n">
         <v>0.0006374641422241191</v>
       </c>
-      <c r="L3" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" t="n">
+      <c r="P3" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="n">
         <v>0.002989396183087676</v>
       </c>
-      <c r="N3" t="n">
+      <c r="R3" t="n">
         <v>-0.002099559230649365</v>
       </c>
-      <c r="O3" t="n">
+      <c r="S3" t="n">
         <v>3.055384884217882e-05</v>
       </c>
-      <c r="P3" t="n">
+      <c r="T3" t="n">
         <v>-0.1314364165195686</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="U3" t="n">
         <v>0.00295579093552271</v>
       </c>
-      <c r="R3" t="n">
+      <c r="V3" t="n">
         <v>0.0001331785678521519</v>
       </c>
-      <c r="S3" t="n">
+      <c r="W3" t="n">
         <v>0.004865215262772999</v>
       </c>
-      <c r="T3" t="n">
+      <c r="X3" t="n">
         <v>0.0001158863554899324</v>
       </c>
-      <c r="U3" t="n">
+      <c r="Y3" t="n">
         <v>0.0006445499573280488</v>
       </c>
-      <c r="V3" t="n">
+      <c r="Z3" t="n">
         <v>-0.001391408972487885</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AA3" t="n">
         <v>0.002034023888948697</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AB3" t="n">
         <v>0.001296547567203661</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="AC3" t="n">
         <v>-0.001178662436239548</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AD3" t="n">
         <v>0.0009634943563493348</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AE3" t="n">
         <v>0.0009281780398005078</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AF3" t="n">
         <v>3.285428518126799e-05</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AG3" t="n">
         <v>0.0001689505001622981</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AH3" t="n">
         <v>0.0004277578257894656</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AI3" t="n">
         <v>0.009979417899159349</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AJ3" t="n">
         <v>0.0003207434226772077</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AK3" t="n">
         <v>0.0006563447694512881</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="AL3" t="n">
         <v>0.001877033209402733</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="AM3" t="n">
         <v>-0.0004311296683697553</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="AN3" t="n">
         <v>6.325027082265683e-06</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="AO3" t="n">
         <v>-0.0009627144707803836</v>
       </c>
     </row>
@@ -7641,108 +7777,120 @@
         <v>-2.779797436360422e-05</v>
       </c>
       <c r="C4" t="n">
+        <v>-0.3532059231582924</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.01290609316766033</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-0.1017071763425346</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
         <v>0.146544873764661</v>
       </c>
-      <c r="D4" t="n">
+      <c r="H4" t="n">
         <v>0.03517625282684171</v>
       </c>
-      <c r="E4" t="n">
+      <c r="I4" t="n">
         <v>0.00446469404745091</v>
       </c>
-      <c r="F4" t="n">
+      <c r="J4" t="n">
         <v>0.09393782022627442</v>
       </c>
-      <c r="G4" t="n">
+      <c r="K4" t="n">
         <v>-0.01869248644095265</v>
       </c>
-      <c r="H4" t="n">
+      <c r="L4" t="n">
         <v>-0.1304735409944164</v>
       </c>
-      <c r="I4" t="n">
+      <c r="M4" t="n">
         <v>0.01476265534508948</v>
       </c>
-      <c r="J4" t="n">
+      <c r="N4" t="n">
         <v>0.001821319967511462</v>
       </c>
-      <c r="K4" t="n">
+      <c r="O4" t="n">
         <v>0.007453498816685515</v>
       </c>
-      <c r="L4" t="n">
+      <c r="P4" t="n">
         <v>-0.004142318872175995</v>
       </c>
-      <c r="M4" t="n">
+      <c r="Q4" t="n">
         <v>-0.04313168939761457</v>
       </c>
-      <c r="N4" t="n">
+      <c r="R4" t="n">
         <v>0.03694838080387918</v>
       </c>
-      <c r="O4" t="n">
+      <c r="S4" t="n">
         <v>0.0002540132293707161</v>
       </c>
-      <c r="P4" t="n">
+      <c r="T4" t="n">
         <v>-0.3615641069656562</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="U4" t="n">
         <v>0.01555710192347452</v>
       </c>
-      <c r="R4" t="n">
+      <c r="V4" t="n">
         <v>-0.1292315091357458</v>
       </c>
-      <c r="S4" t="n">
+      <c r="W4" t="n">
         <v>0.02109230606272237</v>
       </c>
-      <c r="T4" t="n">
+      <c r="X4" t="n">
         <v>-0.008183752440351856</v>
       </c>
-      <c r="U4" t="n">
+      <c r="Y4" t="n">
         <v>-0.002211509167663289</v>
       </c>
-      <c r="V4" t="n">
+      <c r="Z4" t="n">
         <v>-0.01647067882232338</v>
       </c>
-      <c r="W4" t="n">
+      <c r="AA4" t="n">
         <v>0.000439261373722129</v>
       </c>
-      <c r="X4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y4" t="n">
+      <c r="AB4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC4" t="n">
         <v>-0.02594173575934594</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AD4" t="n">
         <v>-0.02810887592231334</v>
       </c>
-      <c r="AA4" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" t="n">
+      <c r="AE4" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="n">
         <v>-0.007608076090592122</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="AG4" t="n">
         <v>-0.01133605301262706</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="AH4" t="n">
         <v>-0.03733751126108776</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AI4" t="n">
         <v>0.01857896548422206</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="AJ4" t="n">
         <v>0.05845300468455671</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="AK4" t="n">
         <v>-0.07902046764506156</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="AL4" t="n">
         <v>-0.02100720046519935</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="AM4" t="n">
         <v>-0.004023343910443228</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="AN4" t="n">
         <v>-0.008816321933428387</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="AO4" t="n">
         <v>-0.0200146212164344</v>
       </c>
     </row>
@@ -7756,108 +7904,120 @@
         <v>0.0002383859446373553</v>
       </c>
       <c r="C5" t="n">
+        <v>-0.2182484002289638</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.001109751869038702</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-0.01557784900746719</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
         <v>-0.05406538531085087</v>
       </c>
-      <c r="D5" t="n">
+      <c r="H5" t="n">
         <v>0.01530579178234035</v>
       </c>
-      <c r="E5" t="n">
+      <c r="I5" t="n">
         <v>0.008281408559996711</v>
       </c>
-      <c r="F5" t="n">
+      <c r="J5" t="n">
         <v>0.03096733500119599</v>
       </c>
-      <c r="G5" t="n">
+      <c r="K5" t="n">
         <v>-0.008990263938727901</v>
       </c>
-      <c r="H5" t="n">
+      <c r="L5" t="n">
         <v>-0.03134684844908651</v>
       </c>
-      <c r="I5" t="n">
+      <c r="M5" t="n">
         <v>-0.005833335661269539</v>
       </c>
-      <c r="J5" t="n">
+      <c r="N5" t="n">
         <v>0.002844663533412643</v>
       </c>
-      <c r="K5" t="n">
+      <c r="O5" t="n">
         <v>0.004786663060144069</v>
       </c>
-      <c r="L5" t="n">
+      <c r="P5" t="n">
         <v>-0.0007550631662699059</v>
       </c>
-      <c r="M5" t="n">
+      <c r="Q5" t="n">
         <v>0.00128744965710946</v>
       </c>
-      <c r="N5" t="n">
+      <c r="R5" t="n">
         <v>0.01806442512583173</v>
       </c>
-      <c r="O5" t="n">
+      <c r="S5" t="n">
         <v>0.0001496976492513098</v>
       </c>
-      <c r="P5" t="n">
+      <c r="T5" t="n">
         <v>-0.2527068185782775</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="U5" t="n">
         <v>0.001575704080222809</v>
       </c>
-      <c r="R5" t="n">
+      <c r="V5" t="n">
         <v>-0.01427838831518643</v>
       </c>
-      <c r="S5" t="n">
+      <c r="W5" t="n">
         <v>0.01564162278332944</v>
       </c>
-      <c r="T5" t="n">
+      <c r="X5" t="n">
         <v>-0.003360996551678146</v>
       </c>
-      <c r="U5" t="n">
+      <c r="Y5" t="n">
         <v>-0.0002772064089065464</v>
       </c>
-      <c r="V5" t="n">
+      <c r="Z5" t="n">
         <v>-0.01192230054467747</v>
       </c>
-      <c r="W5" t="n">
+      <c r="AA5" t="n">
         <v>0.003375511239299751</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AB5" t="n">
         <v>0.005830249646516347</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AC5" t="n">
         <v>-0.01760839868644</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AD5" t="n">
         <v>-0.01124720466895546</v>
       </c>
-      <c r="AA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB5" t="n">
+      <c r="AE5" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF5" t="n">
         <v>-0.003762747324093071</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="AG5" t="n">
         <v>-0.005583757819651318</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AH5" t="n">
         <v>-0.009756019112527197</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AI5" t="n">
         <v>0.006669382302736638</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AJ5" t="n">
         <v>-0.03652543699631138</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AK5" t="n">
         <v>-0.03148007204573314</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="AL5" t="n">
         <v>-0.007498074791951971</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="AM5" t="n">
         <v>-0.002678256752960213</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="AN5" t="n">
         <v>-0.004101667730464453</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AO5" t="n">
         <v>-0.0123465620426252</v>
       </c>
     </row>
@@ -7871,108 +8031,120 @@
         <v>-0.0001306720640153168</v>
       </c>
       <c r="C6" t="n">
+        <v>-0.1739291432736104</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0019606893911018</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-0.002034388085680979</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
         <v>0.02219499424619271</v>
       </c>
-      <c r="D6" t="n">
+      <c r="H6" t="n">
         <v>0.005515848834372472</v>
       </c>
-      <c r="E6" t="n">
+      <c r="I6" t="n">
         <v>0.01413320571956444</v>
       </c>
-      <c r="F6" t="n">
+      <c r="J6" t="n">
         <v>-0.04120463751272746</v>
       </c>
-      <c r="G6" t="n">
+      <c r="K6" t="n">
         <v>-0.003748930577659864</v>
       </c>
-      <c r="H6" t="n">
+      <c r="L6" t="n">
         <v>-0.008413028589473735</v>
       </c>
-      <c r="I6" t="n">
+      <c r="M6" t="n">
         <v>-0.005460070900054078</v>
       </c>
-      <c r="J6" t="n">
+      <c r="N6" t="n">
         <v>0.001640354152333154</v>
       </c>
-      <c r="K6" t="n">
+      <c r="O6" t="n">
         <v>0.003137163313950113</v>
       </c>
-      <c r="L6" t="n">
+      <c r="P6" t="n">
         <v>-0.0003016871112620852</v>
       </c>
-      <c r="M6" t="n">
+      <c r="Q6" t="n">
         <v>-9.508610600770049e-05</v>
       </c>
-      <c r="N6" t="n">
+      <c r="R6" t="n">
         <v>0.009082886690480754</v>
       </c>
-      <c r="O6" t="n">
+      <c r="S6" t="n">
         <v>0.0001287848753260614</v>
       </c>
-      <c r="P6" t="n">
+      <c r="T6" t="n">
         <v>-0.1841431905927917</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="U6" t="n">
         <v>0.004791664388644772</v>
       </c>
-      <c r="R6" t="n">
+      <c r="V6" t="n">
         <v>-0.0006989067723294346</v>
       </c>
-      <c r="S6" t="n">
+      <c r="W6" t="n">
         <v>0.01157234849733694</v>
       </c>
-      <c r="T6" t="n">
+      <c r="X6" t="n">
         <v>-0.001201987803887631</v>
       </c>
-      <c r="U6" t="n">
+      <c r="Y6" t="n">
         <v>0.0009404784744519001</v>
       </c>
-      <c r="V6" t="n">
+      <c r="Z6" t="n">
         <v>-0.006985400303873767</v>
       </c>
-      <c r="W6" t="n">
+      <c r="AA6" t="n">
         <v>0.007228144753164118</v>
       </c>
-      <c r="X6" t="n">
+      <c r="AB6" t="n">
         <v>0.0005587942006646713</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AC6" t="n">
         <v>-0.01205095710818641</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AD6" t="n">
         <v>-0.005304223293643143</v>
       </c>
-      <c r="AA6" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" t="n">
+      <c r="AE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF6" t="n">
         <v>-0.001798259971039246</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AG6" t="n">
         <v>-0.002347041038480885</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AH6" t="n">
         <v>-0.004373286584786283</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AI6" t="n">
         <v>0.005871478759967103</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AJ6" t="n">
         <v>-0.002637805527885299</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AK6" t="n">
         <v>-0.01231322346406158</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="AL6" t="n">
         <v>-0.003557331362086465</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="AM6" t="n">
         <v>-0.001872039906776381</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="AN6" t="n">
         <v>-0.001923416346166064</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="AO6" t="n">
         <v>-0.00689616051987967</v>
       </c>
     </row>
@@ -7986,108 +8158,120 @@
         <v>0.0003498503464228656</v>
       </c>
       <c r="C7" t="n">
+        <v>-0.3490911028167712</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.002422819492199735</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.01251692105802839</v>
       </c>
-      <c r="D7" t="n">
+      <c r="H7" t="n">
         <v>-0.005822618765595726</v>
       </c>
-      <c r="E7" t="n">
+      <c r="I7" t="n">
         <v>0.05624983217322384</v>
       </c>
-      <c r="F7" t="n">
+      <c r="J7" t="n">
         <v>0.001236331905576494</v>
       </c>
-      <c r="G7" t="n">
+      <c r="K7" t="n">
         <v>0.0004646635627893611</v>
       </c>
-      <c r="H7" t="n">
+      <c r="L7" t="n">
         <v>-0.000106863954489181</v>
       </c>
-      <c r="I7" t="n">
+      <c r="M7" t="n">
         <v>-0.009039818292441873</v>
       </c>
-      <c r="J7" t="n">
+      <c r="N7" t="n">
         <v>0.002653722513096692</v>
       </c>
-      <c r="K7" t="n">
+      <c r="O7" t="n">
         <v>6.335977360303261e-05</v>
       </c>
-      <c r="L7" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" t="n">
+      <c r="P7" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="n">
         <v>-0.008414982615948547</v>
       </c>
-      <c r="N7" t="n">
+      <c r="R7" t="n">
         <v>-0.003021839272431629</v>
       </c>
-      <c r="O7" t="n">
+      <c r="S7" t="n">
         <v>0.0007679778214758396</v>
       </c>
-      <c r="P7" t="n">
+      <c r="T7" t="n">
         <v>-0.3330823282167376</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="U7" t="n">
         <v>0.004881672317235436</v>
       </c>
-      <c r="R7" t="n">
+      <c r="V7" t="n">
         <v>0.0002491837028376621</v>
       </c>
-      <c r="S7" t="n">
+      <c r="W7" t="n">
         <v>0.01258754451782542</v>
       </c>
-      <c r="T7" t="n">
+      <c r="X7" t="n">
         <v>0.0001807997783490372</v>
       </c>
-      <c r="U7" t="n">
+      <c r="Y7" t="n">
         <v>0.0003008284578663826</v>
       </c>
-      <c r="V7" t="n">
+      <c r="Z7" t="n">
         <v>-0.006489000829046044</v>
       </c>
-      <c r="W7" t="n">
+      <c r="AA7" t="n">
         <v>0.009252423105117282</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AB7" t="n">
         <v>0.005960918164838301</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AC7" t="n">
         <v>-0.009499941062389796</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AD7" t="n">
         <v>0.0006789498263201894</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AE7" t="n">
         <v>0.00224812796877286</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AF7" t="n">
         <v>-0.0007265944555088497</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AG7" t="n">
         <v>-0.0008239583525776171</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AH7" t="n">
         <v>0.001112805476134028</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AI7" t="n">
         <v>0.01539260326402984</v>
       </c>
-      <c r="AF7" t="n">
+      <c r="AJ7" t="n">
         <v>0.001127627883232733</v>
       </c>
-      <c r="AG7" t="n">
+      <c r="AK7" t="n">
         <v>0.0008144647514063575</v>
       </c>
-      <c r="AH7" t="n">
+      <c r="AL7" t="n">
         <v>-0.001693157451104836</v>
       </c>
-      <c r="AI7" t="n">
+      <c r="AM7" t="n">
         <v>-0.002945554009817732</v>
       </c>
-      <c r="AJ7" t="n">
+      <c r="AN7" t="n">
         <v>-0.0003347092995709501</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="AO7" t="n">
         <v>-0.00488606824832114</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update on subsystem comparison
</commit_message>
<xml_diff>
--- a/Data/ZeLa Data/specific_rates_R.xlsx
+++ b/Data/ZeLa Data/specific_rates_R.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Specific Rates" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg_U1_U3" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Avg_U4_U8" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Int_U1_U3" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Int_U4_U8" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Specific Rates" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Avg_U1_U3" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Avg_U4_U8" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Int_U1_U3" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Int_U4_U8" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -6291,14 +6291,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A20:A25"/>
+    <mergeCell ref="A38:A43"/>
     <mergeCell ref="A2:A7"/>
-    <mergeCell ref="A8:A13"/>
     <mergeCell ref="A14:A19"/>
-    <mergeCell ref="A20:A25"/>
-    <mergeCell ref="A26:A31"/>
+    <mergeCell ref="A44:A49"/>
     <mergeCell ref="A32:A37"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="A44:A49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>